<commit_message>
Sitemaps updates and some corrections
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\vc-docs\sitemap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD24EA-2480-4241-ACBA-9CAFC9749A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6A6CAA-20CE-462C-9742-4179CF03D556}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="docs_virtocommerce_org-sitemap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="265">
   <si>
     <t>Original Url</t>
   </si>
@@ -665,6 +665,156 @@
   </si>
   <si>
     <t>Need to add a new article from previous docs</t>
+  </si>
+  <si>
+    <t>https://help.virtocommerce.com/support/home</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>In the new documentation, the only article about creating new modules is "Creating modules from Template". And its ays it is a recommended way.  Should other ways be described in the new docs?</t>
+  </si>
+  <si>
+    <t>==</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Logging/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Security/extensions/extending-usermanager-and-rolemanager/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Getting-Started/Installation-Guide/windows/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/generating-c-sharp-client/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Back-End-Architecture/02-conceptual-overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Persistence/DB-Agnostic/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Caching/01-overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Modularity/01-overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Security/security-in-depth/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Indexed-Search/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/Extensibility-Points/blade-toolbar/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/Extensibility-Points/blades-and-navigation/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Security/extensions/extending-authorization-policies/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/Tutorials/extending-domain-models/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/Extensibility-Points/extending-grid-columns/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/Extensibility-Points/extending-main-menu/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Event-Driven-Development/using-domain-events/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/Extensibility-Points/metaform/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Payments/new-payment-method-registration/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Shipments/new-shipping-method-registration/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Taxes/new-tax-provider-registration/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Extensibility/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/style-guide/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/ui-scroll-directive/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/Extensibility-Points/widgets/</t>
+  </si>
+  <si>
+    <t>storefront/developer-guide/getting-started/quickstart-on-windows/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Getting-Started/Installation-Guide/macOS/</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Getting-Started/Installation-Guide/linux/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Notifications/overview/</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://virtocommerce.com/open-source-license</t>
+  </si>
+  <si>
+    <t>https://virtostart-demo-admin.govirto.com/docs/index.html</t>
+  </si>
+  <si>
+    <t>https://github.com/VirtoCommerce/vc-platform/releases</t>
+  </si>
+  <si>
+    <t>https://www.virtocommerce.org/c/news-digest/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Security/extensions/adding-new-sso-provider/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Security/configuring-and-managing-azure-auth/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Configuration-Reference/appsettingsjson/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/getting-started/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/security/login-on-behalf/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/modules-installation/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/security/roles-and-permissions/</t>
+  </si>
+  <si>
+    <t>Each described module has a settings section</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>/platform/developer-guide/Fundamentals/Persistence/Concurrency-handling/concurrency-handling/</t>
   </si>
 </sst>
 </file>
@@ -1157,54 +1307,55 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Гиперссылка" xfId="42" builtinId="8"/>
+    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1220,9 +1371,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1260,7 +1411,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1366,7 +1517,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1516,97 +1667,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B213"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="97" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" customWidth="1"/>
+    <col min="2" max="2" width="98.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1614,7 +1813,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1622,7 +1821,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1630,7 +1829,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1638,980 +1837,1601 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C29" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>214</v>
+      </c>
+      <c r="C31" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>214</v>
+      </c>
+      <c r="C57" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>214</v>
+      </c>
+      <c r="C69" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>249</v>
+      </c>
+      <c r="C171" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B172" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B173" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B174" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B175" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B177" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B178" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B179" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B180" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B181" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B182" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
+        <v>249</v>
+      </c>
+      <c r="C183" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B184" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B185" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B186" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B187" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B188" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B189" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B190" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>249</v>
+      </c>
+      <c r="C210" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>213</v>
+      </c>
+      <c r="B213" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A15" r:id="rId2" xr:uid="{1C549BF6-83D2-4C75-AE1D-C2F86A653D1A}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{2F778272-CD26-4C05-A595-DF14512CE623}"/>
+    <hyperlink ref="C29" r:id="rId4" xr:uid="{2F69C9CC-1055-414D-9C75-56CCCD337F48}"/>
+    <hyperlink ref="C171" r:id="rId5" xr:uid="{C639680D-E96B-460A-B8F9-109863FB0F34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add comments to legacy docs rewrite rules (not finished)
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6A6CAA-20CE-462C-9742-4179CF03D556}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C975DC-7094-4575-80D6-27C24625BCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="docs_virtocommerce_org-sitemap" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="272">
   <si>
     <t>Original Url</t>
   </si>
@@ -673,9 +674,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>In the new documentation, the only article about creating new modules is "Creating modules from Template". And its ays it is a recommended way.  Should other ways be described in the new docs?</t>
-  </si>
-  <si>
     <t>==</t>
   </si>
   <si>
@@ -775,9 +773,6 @@
     <t>https://virtocommerce.com/open-source-license</t>
   </si>
   <si>
-    <t>https://virtostart-demo-admin.govirto.com/docs/index.html</t>
-  </si>
-  <si>
     <t>https://github.com/VirtoCommerce/vc-platform/releases</t>
   </si>
   <si>
@@ -815,6 +810,33 @@
   </si>
   <si>
     <t>/platform/developer-guide/Fundamentals/Persistence/Concurrency-handling/concurrency-handling/</t>
+  </si>
+  <si>
+    <t>Legacy article content can combined with this article https://docs2.govirto.com/platform/user-guide/platform-overview/</t>
+  </si>
+  <si>
+    <t>do not move. 301  redirected to docs main page</t>
+  </si>
+  <si>
+    <t>move into /platform/developer-guide/CLI-tools</t>
+  </si>
+  <si>
+    <t>move into /platform/developer-guide/architecture-center</t>
+  </si>
+  <si>
+    <t>In the new documentation, the only article about creating new modules is "Creating modules from Template". And its ays it is a recommended way.  Should other ways be described in the new docs? ET: do not move. Add reditect to Creating modules from Template</t>
+  </si>
+  <si>
+    <t>/platform/developer-guide/CLI-tools</t>
+  </si>
+  <si>
+    <t>move into /platform/developer-guide/Tutorials-and-How-tos/How-tos/modules-development-via-docker/</t>
+  </si>
+  <si>
+    <t>do not move. 301  redirected API REST Api referense</t>
+  </si>
+  <si>
+    <t>301 to platform/developer-guide/Fundamentals/Security/extensions/extending-usermanager-and-rolemanager/</t>
   </si>
 </sst>
 </file>
@@ -1313,49 +1335,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Гиперссылка" xfId="42" builtinId="8"/>
-    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1371,9 +1393,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1411,7 +1433,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1517,7 +1539,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1669,14 +1691,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="97" customWidth="1"/>
-    <col min="2" max="2" width="98.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1700,7 +1722,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1708,10 +1730,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1719,7 +1741,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C5" t="s">
         <v>215</v>
@@ -1730,7 +1752,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1742,11 +1764,14 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>214</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1756,13 +1781,19 @@
       <c r="B9" t="s">
         <v>214</v>
       </c>
+      <c r="C9" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>214</v>
+      </c>
+      <c r="C10" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1772,13 +1803,19 @@
       <c r="B11" t="s">
         <v>214</v>
       </c>
+      <c r="C11" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>214</v>
+      </c>
+      <c r="C12" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1788,13 +1825,19 @@
       <c r="B13" t="s">
         <v>214</v>
       </c>
+      <c r="C13" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>214</v>
+      </c>
+      <c r="C14" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1804,6 +1847,9 @@
       <c r="B15" t="s">
         <v>214</v>
       </c>
+      <c r="C15" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1812,6 +1858,9 @@
       <c r="B16" t="s">
         <v>214</v>
       </c>
+      <c r="C16" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1820,6 +1869,9 @@
       <c r="B17" t="s">
         <v>214</v>
       </c>
+      <c r="C17" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1828,6 +1880,9 @@
       <c r="B18" t="s">
         <v>214</v>
       </c>
+      <c r="C18" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1836,24 +1891,30 @@
       <c r="B19" t="s">
         <v>214</v>
       </c>
+      <c r="C19" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>214</v>
       </c>
+      <c r="C20" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>214</v>
       </c>
       <c r="C21" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1864,7 +1925,7 @@
         <v>214</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1875,7 +1936,7 @@
         <v>214</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1886,7 +1947,7 @@
         <v>214</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1897,15 +1958,18 @@
         <v>214</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>214</v>
+      </c>
+      <c r="C26" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1913,15 +1977,18 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>214</v>
+      </c>
+      <c r="C28" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1932,15 +1999,18 @@
         <v>214</v>
       </c>
       <c r="C29" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="C30" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1951,7 +2021,7 @@
         <v>214</v>
       </c>
       <c r="C31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1959,7 +2029,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1967,7 +2037,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1975,7 +2045,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1983,7 +2053,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1991,7 +2061,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2007,7 +2077,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2015,7 +2085,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2023,7 +2093,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2031,7 +2101,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2039,7 +2109,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2047,7 +2117,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2055,7 +2125,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2063,7 +2133,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2071,7 +2141,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2079,7 +2149,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2087,7 +2157,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -2095,7 +2165,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -2103,7 +2173,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2111,7 +2181,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -2119,7 +2189,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -2135,7 +2205,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2143,7 +2213,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2151,7 +2221,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2162,7 +2232,7 @@
         <v>214</v>
       </c>
       <c r="C57" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2170,7 +2240,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2178,7 +2248,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2186,7 +2256,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2261,7 +2331,7 @@
         <v>214</v>
       </c>
       <c r="C69" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3077,10 +3147,10 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C171" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -3088,7 +3158,7 @@
         <v>172</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -3096,7 +3166,7 @@
         <v>173</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -3104,7 +3174,7 @@
         <v>174</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -3112,7 +3182,7 @@
         <v>175</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -3120,7 +3190,7 @@
         <v>176</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -3128,7 +3198,7 @@
         <v>177</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -3136,7 +3206,7 @@
         <v>178</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -3144,7 +3214,7 @@
         <v>179</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -3152,7 +3222,7 @@
         <v>180</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -3160,7 +3230,7 @@
         <v>181</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -3168,7 +3238,7 @@
         <v>182</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -3176,10 +3246,10 @@
         <v>183</v>
       </c>
       <c r="B183" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C183" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -3187,7 +3257,7 @@
         <v>184</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -3195,7 +3265,7 @@
         <v>185</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -3203,7 +3273,7 @@
         <v>186</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -3211,7 +3281,7 @@
         <v>187</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -3219,7 +3289,7 @@
         <v>188</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -3227,7 +3297,7 @@
         <v>189</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -3235,7 +3305,7 @@
         <v>190</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -3243,7 +3313,7 @@
         <v>191</v>
       </c>
       <c r="B191" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -3251,7 +3321,7 @@
         <v>192</v>
       </c>
       <c r="B192" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3267,7 +3337,7 @@
         <v>194</v>
       </c>
       <c r="B194" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -3355,7 +3425,7 @@
         <v>205</v>
       </c>
       <c r="B205" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -3363,7 +3433,7 @@
         <v>206</v>
       </c>
       <c r="B206" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -3371,7 +3441,7 @@
         <v>207</v>
       </c>
       <c r="B207" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -3379,7 +3449,7 @@
         <v>208</v>
       </c>
       <c r="B208" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -3387,7 +3457,7 @@
         <v>209</v>
       </c>
       <c r="B209" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -3395,10 +3465,10 @@
         <v>210</v>
       </c>
       <c r="B210" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C210" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -3414,7 +3484,7 @@
         <v>212</v>
       </c>
       <c r="B212" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -3422,7 +3492,7 @@
         <v>213</v>
       </c>
       <c r="B213" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3430,8 +3500,18 @@
     <hyperlink ref="A33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A15" r:id="rId2" xr:uid="{1C549BF6-83D2-4C75-AE1D-C2F86A653D1A}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{2F778272-CD26-4C05-A595-DF14512CE623}"/>
-    <hyperlink ref="C29" r:id="rId4" xr:uid="{2F69C9CC-1055-414D-9C75-56CCCD337F48}"/>
+    <hyperlink ref="C29" r:id="rId4" display="https://virtostart-demo-admin.govirto.com/docs/index.html" xr:uid="{2F69C9CC-1055-414D-9C75-56CCCD337F48}"/>
     <hyperlink ref="C171" r:id="rId5" xr:uid="{C639680D-E96B-460A-B8F9-109863FB0F34}"/>
+    <hyperlink ref="A8" r:id="rId6" xr:uid="{9DCA1375-BE25-41A3-BFD5-D458DCF426C1}"/>
+    <hyperlink ref="A10" r:id="rId7" xr:uid="{83DDEF70-B2C9-4E91-A35C-9B12C3EB8B2E}"/>
+    <hyperlink ref="C8" r:id="rId8" display="https://docs2.govirto.com/platform/user-guide/platform-overview/" xr:uid="{54B1457E-C0B2-43A7-AD07-0533B9A43544}"/>
+    <hyperlink ref="A14" r:id="rId9" xr:uid="{9264B295-26F3-44F8-90DF-E6E2685E7F46}"/>
+    <hyperlink ref="A12" r:id="rId10" xr:uid="{E573A631-5089-4D2B-BEB3-17C8C0B96BFC}"/>
+    <hyperlink ref="A20" r:id="rId11" xr:uid="{E71C8A81-B35E-4380-909C-AA136AC252C4}"/>
+    <hyperlink ref="A21" r:id="rId12" xr:uid="{8982B5F7-B733-4675-AEED-94A5C80EFB44}"/>
+    <hyperlink ref="A26" r:id="rId13" xr:uid="{CD5A11FD-E1A4-49C5-AA56-40C0CBAD0DED}"/>
+    <hyperlink ref="A28" r:id="rId14" xr:uid="{682A8677-A276-4D95-8D70-8797E2B3FE60}"/>
+    <hyperlink ref="A30" r:id="rId15" xr:uid="{B40AA49A-6D7B-492B-9552-BC01FA11AE8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update legacy todo list
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59C75C3-7A54-4D5F-8F9C-7F1C5CD8E10D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F3FF3B-5D2B-4819-BE4F-BF98EBCFC82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="docs_virtocommerce_org-sitemap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="367">
   <si>
     <t>Original Url</t>
   </si>
@@ -28,12 +28,6 @@
     <t>New Address</t>
   </si>
   <si>
-    <t>https://docs.virtocommerce.org/sitemap.xml</t>
-  </si>
-  <si>
-    <t>https://docs.virtocommerce.org/</t>
-  </si>
-  <si>
     <t>https://docs.virtocommerce.org/license/</t>
   </si>
   <si>
@@ -772,9 +766,6 @@
     <t>https://virtocommerce.com/open-source-license</t>
   </si>
   <si>
-    <t>https://virtostart-demo-admin.govirto.com/docs/index.html</t>
-  </si>
-  <si>
     <t>https://github.com/VirtoCommerce/vc-platform/releases</t>
   </si>
   <si>
@@ -808,9 +799,6 @@
     <t>Each described module has a settings section</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>platform/user-guide/catalog/overview/</t>
   </si>
   <si>
@@ -850,9 +838,6 @@
     <t>platform/user-guide/catalog/managing-properties/#view-properties</t>
   </si>
   <si>
-    <t>platform/user-guide/catalog-personalization/overview/</t>
-  </si>
-  <si>
     <t>platform/user-guide/content/overview/</t>
   </si>
   <si>
@@ -1028,6 +1013,114 @@
   </si>
   <si>
     <t>platform/user-guide/cart/settings/</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ToDo</t>
+  </si>
+  <si>
+    <t>OnHold</t>
+  </si>
+  <si>
+    <t>Add redirect rule when done</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Eugeney</t>
+  </si>
+  <si>
+    <t>Add redirect</t>
+  </si>
+  <si>
+    <t>Write a new doc</t>
+  </si>
+  <si>
+    <t>Add redirect to platform/developer-guide/CLI-tools</t>
+  </si>
+  <si>
+    <t>Redirect to /platform/developer-guide/Tutorials-and-How-tos/Tutorials/creating-custom-module/</t>
+  </si>
+  <si>
+    <t>Redirect to /platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/</t>
+  </si>
+  <si>
+    <t>Redirect  to platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/</t>
+  </si>
+  <si>
+    <t>Copy content to platform/developer-guide/CLI-tools/build-automation</t>
+  </si>
+  <si>
+    <t>Copy content to platform/developer-guide/CLI-tools/cold-start-and-data-migration</t>
+  </si>
+  <si>
+    <t>Copy content to platform/developer-guide/grab-migrator</t>
+  </si>
+  <si>
+    <t>Copy content to platform/developer-guide/CLI-tools/introduction</t>
+  </si>
+  <si>
+    <t>Copy content to platform/developer-guide/CLI-tools/package-management</t>
+  </si>
+  <si>
+    <t>Copy content to platform/developer-guide/Tutorials-and-How-tos/modules-development-via-docker</t>
+  </si>
+  <si>
+    <t>Copy content to platform/developer-guide/Tutorials-and-How-tos/swagger-endpoints</t>
+  </si>
+  <si>
+    <t>Add redirect when  done</t>
+  </si>
+  <si>
+    <t>Copy content to platform/developer-guide/Scalability/overview</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Dynamic-Properties/overview</t>
+  </si>
+  <si>
+    <t>Copy content to  /platform/user-guide/Assets/overview</t>
+  </si>
+  <si>
+    <t>Create a new artilce /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module</t>
+  </si>
+  <si>
+    <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson1</t>
+  </si>
+  <si>
+    <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson2</t>
+  </si>
+  <si>
+    <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson3</t>
+  </si>
+  <si>
+    <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson4</t>
+  </si>
+  <si>
+    <t>verify and combine with platform/developer-guide/Tutorials-and-How-tos/How-tos/azure-app-configuration/</t>
+  </si>
+  <si>
+    <t>Add content to /platform/developer-guide/Fundamentals/azureblob-assets/</t>
+  </si>
+  <si>
+    <t>/platform/developer-guide/Fundamentals/Indexed-Search/overview/</t>
+  </si>
+  <si>
+    <t>Copy content to platform/user-guide/catalog-publishing/overview/</t>
+  </si>
+  <si>
+    <t>Acomplish with the block for how to user groups propagation works platform/user-guide/catalog-personalization/overview/</t>
+  </si>
+  <si>
+    <t>copy content to platform/developer-guide/Tutorials-and-How-tos/override-rounding-policy</t>
+  </si>
+  <si>
+    <t>copy content to platform/user-guide/contacts/advanced-filter</t>
   </si>
 </sst>
 </file>
@@ -1526,49 +1619,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Гиперссылка" xfId="42" builtinId="8"/>
-    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1584,9 +1677,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1624,7 +1717,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1730,7 +1823,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1872,7 +1965,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1880,19 +1973,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="A231" sqref="A231"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="97" customWidth="1"/>
-    <col min="2" max="2" width="98.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1900,1684 +1996,2749 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+      <c r="D1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C12" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+      <c r="C13" t="s">
+        <v>332</v>
+      </c>
+      <c r="D13" t="s">
+        <v>336</v>
+      </c>
+      <c r="E13" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D14" t="s">
+        <v>336</v>
+      </c>
+      <c r="E14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>346</v>
+      </c>
+      <c r="C15" t="s">
+        <v>332</v>
+      </c>
+      <c r="D15" t="s">
+        <v>336</v>
+      </c>
+      <c r="E15" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+      <c r="C16" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" t="s">
+        <v>336</v>
+      </c>
+      <c r="E16" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+        <v>348</v>
+      </c>
+      <c r="C17" t="s">
+        <v>332</v>
+      </c>
+      <c r="D17" t="s">
+        <v>336</v>
+      </c>
+      <c r="E17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C18" t="s">
+        <v>332</v>
+      </c>
+      <c r="D18" t="s">
+        <v>336</v>
+      </c>
+      <c r="E18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C19" t="s">
+        <v>333</v>
+      </c>
+      <c r="E19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C20" t="s">
+        <v>332</v>
+      </c>
+      <c r="D20" t="s">
+        <v>337</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
-        <v>214</v>
+      <c r="B21" s="1" t="s">
+        <v>342</v>
       </c>
       <c r="C21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+        <v>332</v>
+      </c>
+      <c r="D21" t="s">
+        <v>337</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>214</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B22" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C22" t="s">
+        <v>332</v>
+      </c>
+      <c r="D22" t="s">
+        <v>337</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>214</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+        <v>339</v>
+      </c>
+      <c r="C23" t="s">
+        <v>332</v>
+      </c>
+      <c r="D23" t="s">
+        <v>337</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>214</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+      <c r="C24" t="s">
+        <v>332</v>
+      </c>
+      <c r="D24" t="s">
+        <v>337</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
-      </c>
-      <c r="C25" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C25" t="s">
+        <v>332</v>
+      </c>
+      <c r="D25" t="s">
+        <v>337</v>
+      </c>
+      <c r="E25" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>349</v>
+      </c>
+      <c r="C26" t="s">
+        <v>332</v>
+      </c>
+      <c r="D26" t="s">
+        <v>336</v>
+      </c>
+      <c r="E26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>350</v>
+      </c>
+      <c r="C27" t="s">
+        <v>332</v>
+      </c>
+      <c r="D27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E27" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>332</v>
+      </c>
+      <c r="D28" t="s">
+        <v>337</v>
+      </c>
+      <c r="E28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C29" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+      <c r="D29" t="s">
+        <v>337</v>
+      </c>
+      <c r="E29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+        <v>221</v>
+      </c>
+      <c r="C30" t="s">
+        <v>332</v>
+      </c>
+      <c r="D30" t="s">
+        <v>337</v>
+      </c>
+      <c r="E30" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C31" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+      <c r="D31" t="s">
+        <v>337</v>
+      </c>
+      <c r="E31" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="C32" t="s">
+        <v>332</v>
+      </c>
+      <c r="D32" t="s">
+        <v>337</v>
+      </c>
+      <c r="E32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>332</v>
+      </c>
+      <c r="D33" t="s">
+        <v>337</v>
+      </c>
+      <c r="E33" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C34" t="s">
+        <v>332</v>
+      </c>
+      <c r="D34" t="s">
+        <v>337</v>
+      </c>
+      <c r="E34" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="C35" t="s">
+        <v>332</v>
+      </c>
+      <c r="D35" t="s">
+        <v>336</v>
+      </c>
+      <c r="E35" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="C36" t="s">
+        <v>332</v>
+      </c>
+      <c r="D36" t="s">
+        <v>337</v>
+      </c>
+      <c r="E36" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+      <c r="C37" t="s">
+        <v>332</v>
+      </c>
+      <c r="D37" t="s">
+        <v>337</v>
+      </c>
+      <c r="E37" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>332</v>
+      </c>
+      <c r="D38" t="s">
+        <v>337</v>
+      </c>
+      <c r="E38" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>332</v>
+      </c>
+      <c r="D39" t="s">
+        <v>337</v>
+      </c>
+      <c r="E39" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>332</v>
+      </c>
+      <c r="D40" t="s">
+        <v>337</v>
+      </c>
+      <c r="E40" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>332</v>
+      </c>
+      <c r="D41" t="s">
+        <v>337</v>
+      </c>
+      <c r="E41" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>332</v>
+      </c>
+      <c r="D42" t="s">
+        <v>337</v>
+      </c>
+      <c r="E42" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>332</v>
+      </c>
+      <c r="D43" t="s">
+        <v>337</v>
+      </c>
+      <c r="E43" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>332</v>
+      </c>
+      <c r="D44" t="s">
+        <v>337</v>
+      </c>
+      <c r="E44" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>332</v>
+      </c>
+      <c r="D45" t="s">
+        <v>337</v>
+      </c>
+      <c r="E45" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>332</v>
+      </c>
+      <c r="D46" t="s">
+        <v>337</v>
+      </c>
+      <c r="E46" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>332</v>
+      </c>
+      <c r="D47" t="s">
+        <v>337</v>
+      </c>
+      <c r="E47" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>332</v>
+      </c>
+      <c r="D48" t="s">
+        <v>337</v>
+      </c>
+      <c r="E48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>332</v>
+      </c>
+      <c r="D49" t="s">
+        <v>337</v>
+      </c>
+      <c r="E49" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="C50" t="s">
+        <v>332</v>
+      </c>
+      <c r="D50" t="s">
+        <v>337</v>
+      </c>
+      <c r="E50" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="C51" t="s">
+        <v>332</v>
+      </c>
+      <c r="D51" t="s">
+        <v>337</v>
+      </c>
+      <c r="E51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="C52" t="s">
+        <v>332</v>
+      </c>
+      <c r="D52" t="s">
+        <v>337</v>
+      </c>
+      <c r="E52" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="C53" t="s">
+        <v>332</v>
+      </c>
+      <c r="D53" t="s">
+        <v>337</v>
+      </c>
+      <c r="E53" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>332</v>
+      </c>
+      <c r="D54" t="s">
+        <v>337</v>
+      </c>
+      <c r="E54" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+      <c r="C55" t="s">
+        <v>332</v>
+      </c>
+      <c r="D55" t="s">
+        <v>337</v>
+      </c>
+      <c r="E55" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="C56" t="s">
+        <v>332</v>
+      </c>
+      <c r="D56" t="s">
+        <v>337</v>
+      </c>
+      <c r="E56" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="C57" t="s">
+        <v>332</v>
+      </c>
+      <c r="D57" t="s">
+        <v>337</v>
+      </c>
+      <c r="E57" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+        <v>245</v>
+      </c>
+      <c r="C58" t="s">
+        <v>332</v>
+      </c>
+      <c r="D58" t="s">
+        <v>337</v>
+      </c>
+      <c r="E58" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+        <v>355</v>
+      </c>
+      <c r="C59" t="s">
+        <v>332</v>
+      </c>
+      <c r="D59" t="s">
+        <v>336</v>
+      </c>
+      <c r="E59" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="C60" t="s">
+        <v>332</v>
+      </c>
+      <c r="D60" t="s">
+        <v>336</v>
+      </c>
+      <c r="E60" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+      <c r="C61" t="s">
+        <v>332</v>
+      </c>
+      <c r="D61" t="s">
+        <v>336</v>
+      </c>
+      <c r="E61" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="C62" t="s">
+        <v>332</v>
+      </c>
+      <c r="D62" t="s">
+        <v>336</v>
+      </c>
+      <c r="E62" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+        <v>359</v>
+      </c>
+      <c r="C63" t="s">
+        <v>332</v>
+      </c>
+      <c r="D63" t="s">
+        <v>336</v>
+      </c>
+      <c r="E63" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+        <v>354</v>
+      </c>
+      <c r="C64" t="s">
+        <v>332</v>
+      </c>
+      <c r="D64" t="s">
+        <v>336</v>
+      </c>
+      <c r="E64" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+        <v>360</v>
+      </c>
+      <c r="C65" t="s">
+        <v>332</v>
+      </c>
+      <c r="D65" t="s">
+        <v>336</v>
+      </c>
+      <c r="E65" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+      <c r="C66" t="s">
+        <v>332</v>
+      </c>
+      <c r="D66" t="s">
+        <v>336</v>
+      </c>
+      <c r="E66" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="C67" t="s">
+        <v>332</v>
+      </c>
+      <c r="D67" t="s">
+        <v>337</v>
+      </c>
+      <c r="E67" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="C68" t="s">
+        <v>332</v>
+      </c>
+      <c r="D68" t="s">
+        <v>337</v>
+      </c>
+      <c r="E68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="C69" t="s">
+        <v>332</v>
+      </c>
+      <c r="D69" t="s">
+        <v>337</v>
+      </c>
+      <c r="E69" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="C70" t="s">
+        <v>332</v>
+      </c>
+      <c r="D70" t="s">
+        <v>337</v>
+      </c>
+      <c r="E70" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="C71" t="s">
+        <v>332</v>
+      </c>
+      <c r="D71" t="s">
+        <v>337</v>
+      </c>
+      <c r="E71" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="C72" t="s">
+        <v>332</v>
+      </c>
+      <c r="D72" t="s">
+        <v>337</v>
+      </c>
+      <c r="E72" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="C73" t="s">
+        <v>332</v>
+      </c>
+      <c r="D73" t="s">
+        <v>337</v>
+      </c>
+      <c r="E73" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="C74" t="s">
+        <v>332</v>
+      </c>
+      <c r="D74" t="s">
+        <v>337</v>
+      </c>
+      <c r="E74" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="C75" t="s">
+        <v>332</v>
+      </c>
+      <c r="D75" t="s">
+        <v>337</v>
+      </c>
+      <c r="E75" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+      <c r="C76" t="s">
+        <v>332</v>
+      </c>
+      <c r="D76" t="s">
+        <v>337</v>
+      </c>
+      <c r="E76" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
-      <c r="B77" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C77" t="s">
+        <v>332</v>
+      </c>
+      <c r="D77" t="s">
+        <v>337</v>
+      </c>
+      <c r="E77" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+        <v>268</v>
+      </c>
+      <c r="C78" t="s">
+        <v>332</v>
+      </c>
+      <c r="D78" t="s">
+        <v>337</v>
+      </c>
+      <c r="E78" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>362</v>
+      </c>
+      <c r="C79" t="s">
+        <v>332</v>
+      </c>
+      <c r="D79" t="s">
+        <v>337</v>
+      </c>
+      <c r="E79" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+      <c r="C80" t="s">
+        <v>332</v>
+      </c>
+      <c r="D80" t="s">
+        <v>337</v>
+      </c>
+      <c r="E80" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="C81" t="s">
+        <v>332</v>
+      </c>
+      <c r="D81" t="s">
+        <v>337</v>
+      </c>
+      <c r="E81" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="C82" t="s">
+        <v>332</v>
+      </c>
+      <c r="D82" t="s">
+        <v>337</v>
+      </c>
+      <c r="E82" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+        <v>364</v>
+      </c>
+      <c r="C83" t="s">
+        <v>332</v>
+      </c>
+      <c r="D83" t="s">
+        <v>336</v>
+      </c>
+      <c r="E83" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+      <c r="C84" t="s">
+        <v>332</v>
+      </c>
+      <c r="D84" t="s">
+        <v>336</v>
+      </c>
+      <c r="E84" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+      <c r="C85" t="s">
+        <v>332</v>
+      </c>
+      <c r="D85" t="s">
+        <v>337</v>
+      </c>
+      <c r="E85" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+      <c r="C86" t="s">
+        <v>332</v>
+      </c>
+      <c r="D86" t="s">
+        <v>337</v>
+      </c>
+      <c r="E86" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+      <c r="C87" t="s">
+        <v>332</v>
+      </c>
+      <c r="D87" t="s">
+        <v>337</v>
+      </c>
+      <c r="E87" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+      <c r="C88" t="s">
+        <v>332</v>
+      </c>
+      <c r="D88" t="s">
+        <v>337</v>
+      </c>
+      <c r="E88" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+        <v>276</v>
+      </c>
+      <c r="C89" t="s">
+        <v>332</v>
+      </c>
+      <c r="D89" t="s">
+        <v>337</v>
+      </c>
+      <c r="E89" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+      <c r="C90" t="s">
+        <v>332</v>
+      </c>
+      <c r="D90" t="s">
+        <v>336</v>
+      </c>
+      <c r="E90" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+        <v>277</v>
+      </c>
+      <c r="C91" t="s">
+        <v>332</v>
+      </c>
+      <c r="D91" t="s">
+        <v>337</v>
+      </c>
+      <c r="E91" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+      <c r="C92" t="s">
+        <v>332</v>
+      </c>
+      <c r="D92" t="s">
+        <v>336</v>
+      </c>
+      <c r="E92" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="C93" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="C94" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="C95" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="C96" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="C97" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C98" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C99" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C100" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+      <c r="C101" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C102" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C103" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C104" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C105" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C106" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="C107" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C108" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="C109" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+      <c r="C110" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="C111" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="C112" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="C113" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="C114" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+      <c r="C115" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="C116" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="C117" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C118" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="C119" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+      <c r="C120" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="C121" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+      <c r="C122" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+      <c r="C123" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+      <c r="C124" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+      <c r="C125" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="C126" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="C127" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="C128" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="C129" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="C130" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+      <c r="C131" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="C132" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+      <c r="C133" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C134" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="C135" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+      <c r="C136" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+      <c r="C137" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+      <c r="C138" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+      <c r="C139" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="C140" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+      <c r="C141" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+      <c r="C142" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="C143" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="C144" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+      <c r="C145" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+      <c r="C146" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>147</v>
       </c>
       <c r="B147" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="C147" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+      <c r="C148" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="C149" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+      <c r="C150" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>151</v>
       </c>
       <c r="B151" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="C151" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+      <c r="C152" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>153</v>
       </c>
       <c r="B153" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="C153" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>154</v>
       </c>
       <c r="B154" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="C154" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>155</v>
       </c>
       <c r="B155" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+      <c r="C155" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>156</v>
       </c>
       <c r="B156" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+      <c r="C156" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>157</v>
       </c>
       <c r="B157" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="C157" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>158</v>
       </c>
       <c r="B158" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C158" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>159</v>
       </c>
       <c r="B159" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+      <c r="C159" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>160</v>
       </c>
       <c r="B160" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C160" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>161</v>
       </c>
       <c r="B161" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+      <c r="C161" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>162</v>
       </c>
       <c r="B162" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+      <c r="C162" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>163</v>
       </c>
       <c r="B163" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+      <c r="C163" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>164</v>
       </c>
       <c r="B164" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C164" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>165</v>
       </c>
       <c r="B165" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+      <c r="C165" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>166</v>
       </c>
       <c r="B166" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C166" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>167</v>
       </c>
       <c r="B167" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C167" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>168</v>
       </c>
       <c r="B168" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C168" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C169" t="s">
+        <v>332</v>
+      </c>
+      <c r="E169" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C170" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C171" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C172" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C173" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C174" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C175" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C176" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C177" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>178</v>
       </c>
       <c r="B178" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C178" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C179" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="C180" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>181</v>
       </c>
       <c r="B181" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="C181" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>182</v>
       </c>
-      <c r="B182" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B182" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C182" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>183</v>
       </c>
-      <c r="B183" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B183" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C183" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>184</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="C184" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>185</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="C185" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>186</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="C186" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>187</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="C187" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>188</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="C188" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>189</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
+        <v>250</v>
+      </c>
+      <c r="C189" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>190</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
+        <v>251</v>
+      </c>
+      <c r="C190" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>191</v>
       </c>
       <c r="B191" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C191" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>192</v>
       </c>
       <c r="B192" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="C192" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>193</v>
       </c>
       <c r="B193" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C193" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>194</v>
       </c>
       <c r="B194" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C194" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>195</v>
       </c>
       <c r="B195" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C195" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>196</v>
       </c>
       <c r="B196" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C196" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>197</v>
       </c>
       <c r="B197" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C197" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>198</v>
       </c>
       <c r="B198" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+      <c r="C198" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>199</v>
       </c>
       <c r="B199" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C199" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>200</v>
       </c>
       <c r="B200" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C200" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>201</v>
       </c>
       <c r="B201" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C201" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>202</v>
       </c>
       <c r="B202" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="C202" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>203</v>
       </c>
       <c r="B203" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="C203" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>204</v>
       </c>
       <c r="B204" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="C204" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>205</v>
       </c>
       <c r="B205" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="C205" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>206</v>
       </c>
       <c r="B206" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="C206" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>207</v>
       </c>
       <c r="B207" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="C207" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>208</v>
       </c>
       <c r="B208" t="s">
-        <v>259</v>
+        <v>246</v>
+      </c>
+      <c r="C208" t="s">
+        <v>332</v>
+      </c>
+      <c r="E208" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -3585,7 +4746,10 @@
         <v>209</v>
       </c>
       <c r="B209" t="s">
-        <v>260</v>
+        <v>212</v>
+      </c>
+      <c r="C209" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -3593,10 +4757,10 @@
         <v>210</v>
       </c>
       <c r="B210" t="s">
-        <v>248</v>
+        <v>329</v>
       </c>
       <c r="C210" t="s">
-        <v>261</v>
+        <v>332</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -3604,32 +4768,51 @@
         <v>211</v>
       </c>
       <c r="B211" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>212</v>
-      </c>
-      <c r="B212" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>213</v>
-      </c>
-      <c r="B213" t="s">
-        <v>334</v>
+        <v>329</v>
+      </c>
+      <c r="C211" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D211" xr:uid="{85BA2441-4314-49BC-959A-43D8DA1A17A7}">
+      <formula1>"Maria,Eugeney"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C211" xr:uid="{B256EAF5-3172-48AB-8E3F-6AAE55F61A51}">
+      <formula1>"ToDo,OnHold,Completed,Active,OnReview"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A15" r:id="rId2" xr:uid="{1C549BF6-83D2-4C75-AE1D-C2F86A653D1A}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{2F778272-CD26-4C05-A595-DF14512CE623}"/>
-    <hyperlink ref="C29" r:id="rId4" xr:uid="{2F69C9CC-1055-414D-9C75-56CCCD337F48}"/>
-    <hyperlink ref="C171" r:id="rId5" xr:uid="{C639680D-E96B-460A-B8F9-109863FB0F34}"/>
+    <hyperlink ref="A31" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{1C549BF6-83D2-4C75-AE1D-C2F86A653D1A}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{2F778272-CD26-4C05-A595-DF14512CE623}"/>
+    <hyperlink ref="E27" r:id="rId4" display="https://virtostart-demo-admin.govirto.com/docs/index.html" xr:uid="{2F69C9CC-1055-414D-9C75-56CCCD337F48}"/>
+    <hyperlink ref="E169" r:id="rId5" xr:uid="{C639680D-E96B-460A-B8F9-109863FB0F34}"/>
+    <hyperlink ref="A18" r:id="rId6" xr:uid="{3EE074AE-E7B4-410B-995E-14E385EBD9D9}"/>
+    <hyperlink ref="A20" r:id="rId7" xr:uid="{A846E1E7-1C10-438C-8D77-B29FB7B9DDCB}"/>
+    <hyperlink ref="B20" r:id="rId8" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/Tutorials/creating-custom-module/" xr:uid="{20723581-A5B8-40ED-9B17-3E77BBDED0EE}"/>
+    <hyperlink ref="A21" r:id="rId9" xr:uid="{13623968-93F4-4187-901B-4CBAB89D76F0}"/>
+    <hyperlink ref="B21" r:id="rId10" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/" xr:uid="{E30A31FF-1C73-4CA9-A021-B80BED4646E7}"/>
+    <hyperlink ref="A22" r:id="rId11" xr:uid="{0E681307-BB1C-4BD8-8A9E-5044EC1C59B6}"/>
+    <hyperlink ref="B22" r:id="rId12" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/" xr:uid="{AA700B5F-11D7-4E1E-9611-FE738BEF6BC4}"/>
+    <hyperlink ref="A23" r:id="rId13" xr:uid="{D676FAF4-1680-4AE0-B48E-4C1F894CC542}"/>
+    <hyperlink ref="A24" r:id="rId14" xr:uid="{51CA47E3-9EDA-4F3F-9A20-DA44C4B36016}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{EBD2BA40-D76F-4105-B6BA-313C8046E566}"/>
+    <hyperlink ref="A26" r:id="rId16" xr:uid="{736CF484-2649-4C60-BDBD-AA3027BC4179}"/>
+    <hyperlink ref="A27" r:id="rId17" xr:uid="{7BD62CB9-4B34-45EF-911B-C961E0490377}"/>
+    <hyperlink ref="A28" r:id="rId18" xr:uid="{A76A15B9-FDDE-49A2-9A79-B78E65D68304}"/>
+    <hyperlink ref="A35" r:id="rId19" xr:uid="{7FE9D0BF-2813-442F-9B0A-E1D382D595B0}"/>
+    <hyperlink ref="A51" r:id="rId20" xr:uid="{B085393A-1208-4897-8C53-B853C7A540DA}"/>
+    <hyperlink ref="A59" r:id="rId21" xr:uid="{C9E5A96B-07CA-4609-B494-FFD7139FF80F}"/>
+    <hyperlink ref="A64" r:id="rId22" xr:uid="{0D02B00C-8889-41AD-A5C7-868F266E5D07}"/>
+    <hyperlink ref="A60" r:id="rId23" xr:uid="{728667AF-BEB9-41A4-A80B-FBD8B37A60E0}"/>
+    <hyperlink ref="A65" r:id="rId24" xr:uid="{E5E95940-AF1C-4DD9-A0B1-14074CE6C427}"/>
+    <hyperlink ref="A66" r:id="rId25" xr:uid="{1C5554FC-04EC-47BC-89DB-1728DBAE98CB}"/>
+    <hyperlink ref="A79" r:id="rId26" xr:uid="{D8CF9C4B-F15C-4E37-AA00-9F1BFEA56A7E}"/>
+    <hyperlink ref="A84" r:id="rId27" xr:uid="{4FBB0E83-5DCD-436A-94D0-3D97C5F74AA0}"/>
+    <hyperlink ref="A90" r:id="rId28" xr:uid="{0B30FCB3-A6B1-481B-B95C-3C058F657A36}"/>
+    <hyperlink ref="A92" r:id="rId29" xr:uid="{D4EA3FF3-9912-4F0B-BB5E-F0FD06FBC453}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Storefront updates, File Upload section added, Versions section added
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\vc-docs\sitemap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F3FF3B-5D2B-4819-BE4F-BF98EBCFC82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741EEC35-9196-477E-A816-D255DFD088D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="docs_virtocommerce_org-sitemap" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="380">
   <si>
     <t>Original Url</t>
   </si>
@@ -1054,21 +1054,6 @@
     <t>Redirect  to platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/</t>
   </si>
   <si>
-    <t>Copy content to platform/developer-guide/CLI-tools/build-automation</t>
-  </si>
-  <si>
-    <t>Copy content to platform/developer-guide/CLI-tools/cold-start-and-data-migration</t>
-  </si>
-  <si>
-    <t>Copy content to platform/developer-guide/grab-migrator</t>
-  </si>
-  <si>
-    <t>Copy content to platform/developer-guide/CLI-tools/introduction</t>
-  </si>
-  <si>
-    <t>Copy content to platform/developer-guide/CLI-tools/package-management</t>
-  </si>
-  <si>
     <t>Copy content to platform/developer-guide/Tutorials-and-How-tos/modules-development-via-docker</t>
   </si>
   <si>
@@ -1121,6 +1106,60 @@
   </si>
   <si>
     <t>copy content to platform/user-guide/contacts/advanced-filter</t>
+  </si>
+  <si>
+    <t>OnReview</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/CLI-tools/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/CLI-tools/cold-start-data-migration/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/CLI-tools/package-management/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/CLI-tools/build-automation/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/CLI-tools/grab-migrator/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/virto3-products-versions/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2020-Q3/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2021-Q1/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2021-Q3/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2022-Q1/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2022-Q2/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2022-Q3/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2022-Q4/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2023-S5/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2023-S6/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2024-S7/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/versions/v3-2024-S8/</t>
   </si>
 </sst>
 </file>
@@ -1619,49 +1658,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Гиперссылка" xfId="42" builtinId="8"/>
+    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1677,9 +1716,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1717,7 +1756,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1823,7 +1862,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1965,7 +2004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1975,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,10 +2146,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="C13" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
       <c r="D13" t="s">
         <v>336</v>
@@ -2124,10 +2163,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>345</v>
+        <v>364</v>
       </c>
       <c r="C14" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
       <c r="D14" t="s">
         <v>336</v>
@@ -2141,10 +2180,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="C15" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
       <c r="D15" t="s">
         <v>336</v>
@@ -2158,10 +2197,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="C16" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
       <c r="D16" t="s">
         <v>336</v>
@@ -2175,10 +2214,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>365</v>
       </c>
       <c r="C17" t="s">
-        <v>332</v>
+        <v>362</v>
       </c>
       <c r="D17" t="s">
         <v>336</v>
@@ -2325,7 +2364,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="C26" t="s">
         <v>332</v>
@@ -2342,7 +2381,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C27" t="s">
         <v>332</v>
@@ -2351,7 +2390,7 @@
         <v>336</v>
       </c>
       <c r="E27" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2478,7 +2517,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C35" t="s">
         <v>332</v>
@@ -2750,7 +2789,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C51" t="s">
         <v>332</v>
@@ -2886,7 +2925,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="C59" t="s">
         <v>332</v>
@@ -2895,7 +2934,7 @@
         <v>336</v>
       </c>
       <c r="E59" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2903,7 +2942,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="C60" t="s">
         <v>332</v>
@@ -2912,7 +2951,7 @@
         <v>336</v>
       </c>
       <c r="E60" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2920,7 +2959,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C61" t="s">
         <v>332</v>
@@ -2929,7 +2968,7 @@
         <v>336</v>
       </c>
       <c r="E61" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2937,7 +2976,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C62" t="s">
         <v>332</v>
@@ -2946,7 +2985,7 @@
         <v>336</v>
       </c>
       <c r="E62" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2954,7 +2993,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C63" t="s">
         <v>332</v>
@@ -2963,7 +3002,7 @@
         <v>336</v>
       </c>
       <c r="E63" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2971,7 +3010,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C64" t="s">
         <v>332</v>
@@ -2980,7 +3019,7 @@
         <v>336</v>
       </c>
       <c r="E64" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2988,7 +3027,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C65" t="s">
         <v>332</v>
@@ -2997,7 +3036,7 @@
         <v>336</v>
       </c>
       <c r="E65" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3005,7 +3044,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C66" t="s">
         <v>332</v>
@@ -3014,7 +3053,7 @@
         <v>336</v>
       </c>
       <c r="E66" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3226,7 +3265,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C79" t="s">
         <v>332</v>
@@ -3294,7 +3333,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C83" t="s">
         <v>332</v>
@@ -3303,7 +3342,7 @@
         <v>336</v>
       </c>
       <c r="E83" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3311,7 +3350,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C84" t="s">
         <v>332</v>
@@ -3320,7 +3359,7 @@
         <v>336</v>
       </c>
       <c r="E84" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3413,7 +3452,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C90" t="s">
         <v>332</v>
@@ -3422,7 +3461,7 @@
         <v>336</v>
       </c>
       <c r="E90" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3447,7 +3486,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C92" t="s">
         <v>332</v>
@@ -3456,7 +3495,7 @@
         <v>336</v>
       </c>
       <c r="E92" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4300,10 +4339,13 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>329</v>
+        <v>368</v>
       </c>
       <c r="C169" t="s">
-        <v>332</v>
+        <v>362</v>
+      </c>
+      <c r="D169" t="s">
+        <v>336</v>
       </c>
       <c r="E169" t="s">
         <v>248</v>
@@ -4314,10 +4356,13 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>329</v>
+        <v>369</v>
       </c>
       <c r="C170" t="s">
-        <v>332</v>
+        <v>362</v>
+      </c>
+      <c r="D170" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4325,10 +4370,13 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>329</v>
+        <v>370</v>
       </c>
       <c r="C171" t="s">
-        <v>332</v>
+        <v>362</v>
+      </c>
+      <c r="D171" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4336,10 +4384,13 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>329</v>
+        <v>371</v>
       </c>
       <c r="C172" t="s">
-        <v>332</v>
+        <v>362</v>
+      </c>
+      <c r="D172" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4347,10 +4398,13 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>329</v>
+        <v>372</v>
       </c>
       <c r="C173" t="s">
-        <v>332</v>
+        <v>362</v>
+      </c>
+      <c r="D173" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4358,10 +4412,13 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>329</v>
+        <v>373</v>
       </c>
       <c r="C174" t="s">
-        <v>332</v>
+        <v>362</v>
+      </c>
+      <c r="D174" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4369,10 +4426,13 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>329</v>
+        <v>374</v>
       </c>
       <c r="C175" t="s">
-        <v>332</v>
+        <v>362</v>
+      </c>
+      <c r="D175" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4380,57 +4440,72 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>329</v>
+        <v>375</v>
       </c>
       <c r="C176" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+      <c r="D176" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>329</v>
+        <v>376</v>
       </c>
       <c r="C177" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+      <c r="D177" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>178</v>
       </c>
-      <c r="B178" t="s">
-        <v>329</v>
+      <c r="B178" s="1" t="s">
+        <v>377</v>
       </c>
       <c r="C178" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+      <c r="D178" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>329</v>
+        <v>378</v>
       </c>
       <c r="C179" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+      <c r="D179" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>329</v>
+        <v>379</v>
       </c>
       <c r="C180" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+      <c r="D180" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>181</v>
       </c>
@@ -4441,7 +4516,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>182</v>
       </c>
@@ -4452,7 +4527,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>183</v>
       </c>
@@ -4463,7 +4538,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>184</v>
       </c>
@@ -4474,7 +4549,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>185</v>
       </c>
@@ -4485,7 +4560,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>186</v>
       </c>
@@ -4496,7 +4571,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>187</v>
       </c>
@@ -4507,7 +4582,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>188</v>
       </c>
@@ -4518,7 +4593,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>189</v>
       </c>
@@ -4529,7 +4604,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>190</v>
       </c>
@@ -4540,7 +4615,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>191</v>
       </c>
@@ -4551,7 +4626,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
Corrected links, added articles for redirection purposes,
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741EEC35-9196-477E-A816-D255DFD088D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB127F28-95A7-4774-BE31-BE0C1B8EA3BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="381">
   <si>
     <t>Original Url</t>
   </si>
@@ -1054,12 +1054,6 @@
     <t>Redirect  to platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/</t>
   </si>
   <si>
-    <t>Copy content to platform/developer-guide/Tutorials-and-How-tos/modules-development-via-docker</t>
-  </si>
-  <si>
-    <t>Copy content to platform/developer-guide/Tutorials-and-How-tos/swagger-endpoints</t>
-  </si>
-  <si>
     <t>Add redirect when  done</t>
   </si>
   <si>
@@ -1160,6 +1154,15 @@
   </si>
   <si>
     <t>platform/user-guide/versions/v3-2024-S8/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/multiregional-ecommerce/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/swagger-api/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/docker-modules-development/</t>
   </si>
 </sst>
 </file>
@@ -2014,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,10 +2149,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D13" t="s">
         <v>336</v>
@@ -2163,10 +2166,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D14" t="s">
         <v>336</v>
@@ -2180,10 +2183,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D15" t="s">
         <v>336</v>
@@ -2197,10 +2200,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D16" t="s">
         <v>336</v>
@@ -2214,10 +2217,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C17" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D17" t="s">
         <v>336</v>
@@ -2231,10 +2234,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>378</v>
       </c>
       <c r="C18" t="s">
-        <v>332</v>
+        <v>360</v>
       </c>
       <c r="D18" t="s">
         <v>336</v>
@@ -2364,10 +2367,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>344</v>
+        <v>380</v>
       </c>
       <c r="C26" t="s">
-        <v>332</v>
+        <v>360</v>
       </c>
       <c r="D26" t="s">
         <v>336</v>
@@ -2381,16 +2384,16 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>345</v>
+        <v>379</v>
       </c>
       <c r="C27" t="s">
-        <v>332</v>
+        <v>360</v>
       </c>
       <c r="D27" t="s">
         <v>336</v>
       </c>
       <c r="E27" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2517,7 +2520,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C35" t="s">
         <v>332</v>
@@ -2789,7 +2792,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C51" t="s">
         <v>332</v>
@@ -2925,7 +2928,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C59" t="s">
         <v>332</v>
@@ -2934,7 +2937,7 @@
         <v>336</v>
       </c>
       <c r="E59" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2942,7 +2945,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C60" t="s">
         <v>332</v>
@@ -2951,7 +2954,7 @@
         <v>336</v>
       </c>
       <c r="E60" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2959,7 +2962,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C61" t="s">
         <v>332</v>
@@ -2968,7 +2971,7 @@
         <v>336</v>
       </c>
       <c r="E61" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2976,7 +2979,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C62" t="s">
         <v>332</v>
@@ -2985,7 +2988,7 @@
         <v>336</v>
       </c>
       <c r="E62" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2993,7 +2996,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C63" t="s">
         <v>332</v>
@@ -3002,7 +3005,7 @@
         <v>336</v>
       </c>
       <c r="E63" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3010,7 +3013,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C64" t="s">
         <v>332</v>
@@ -3019,7 +3022,7 @@
         <v>336</v>
       </c>
       <c r="E64" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3027,7 +3030,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C65" t="s">
         <v>332</v>
@@ -3036,7 +3039,7 @@
         <v>336</v>
       </c>
       <c r="E65" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3044,7 +3047,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C66" t="s">
         <v>332</v>
@@ -3053,7 +3056,7 @@
         <v>336</v>
       </c>
       <c r="E66" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3265,7 +3268,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C79" t="s">
         <v>332</v>
@@ -3333,7 +3336,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C83" t="s">
         <v>332</v>
@@ -3342,7 +3345,7 @@
         <v>336</v>
       </c>
       <c r="E83" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3350,7 +3353,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C84" t="s">
         <v>332</v>
@@ -3359,7 +3362,7 @@
         <v>336</v>
       </c>
       <c r="E84" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3452,7 +3455,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C90" t="s">
         <v>332</v>
@@ -3461,7 +3464,7 @@
         <v>336</v>
       </c>
       <c r="E90" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3486,7 +3489,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C92" t="s">
         <v>332</v>
@@ -3495,7 +3498,7 @@
         <v>336</v>
       </c>
       <c r="E92" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4339,10 +4342,10 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C169" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D169" t="s">
         <v>336</v>
@@ -4356,10 +4359,10 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C170" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D170" t="s">
         <v>336</v>
@@ -4370,10 +4373,10 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C171" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D171" t="s">
         <v>336</v>
@@ -4384,10 +4387,10 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C172" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D172" t="s">
         <v>336</v>
@@ -4398,10 +4401,10 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C173" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D173" t="s">
         <v>336</v>
@@ -4412,10 +4415,10 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C174" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D174" t="s">
         <v>336</v>
@@ -4426,10 +4429,10 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C175" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D175" t="s">
         <v>336</v>
@@ -4440,10 +4443,10 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C176" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D176" t="s">
         <v>336</v>
@@ -4454,10 +4457,10 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C177" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D177" t="s">
         <v>336</v>
@@ -4468,10 +4471,10 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C178" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D178" t="s">
         <v>336</v>
@@ -4482,10 +4485,10 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C179" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D179" t="s">
         <v>336</v>
@@ -4496,10 +4499,10 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C180" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D180" t="s">
         <v>336</v>

</xml_diff>

<commit_message>
Assets and Skyflow sections added, Azure ad articles updated, Creating new module from scratch article added
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB127F28-95A7-4774-BE31-BE0C1B8EA3BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DD8F75-AF9C-4FCC-913F-ED1E4C34FC31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1063,9 +1063,6 @@
     <t>platform/developer-guide/Fundamentals/Dynamic-Properties/overview</t>
   </si>
   <si>
-    <t>Copy content to  /platform/user-guide/Assets/overview</t>
-  </si>
-  <si>
     <t>Create a new artilce /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module</t>
   </si>
   <si>
@@ -1081,12 +1078,6 @@
     <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson4</t>
   </si>
   <si>
-    <t>verify and combine with platform/developer-guide/Tutorials-and-How-tos/How-tos/azure-app-configuration/</t>
-  </si>
-  <si>
-    <t>Add content to /platform/developer-guide/Fundamentals/azureblob-assets/</t>
-  </si>
-  <si>
     <t>/platform/developer-guide/Fundamentals/Indexed-Search/overview/</t>
   </si>
   <si>
@@ -1163,6 +1154,15 @@
   </si>
   <si>
     <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/docker-modules-development/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/Tutorials/create-new-module-from-scratch/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/assets/managing-assets/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Configuration-Reference/appsettingsjson/#__tabbed_2_2</t>
   </si>
 </sst>
 </file>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,10 +2149,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C13" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D13" t="s">
         <v>336</v>
@@ -2166,10 +2166,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C14" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D14" t="s">
         <v>336</v>
@@ -2183,10 +2183,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C15" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D15" t="s">
         <v>336</v>
@@ -2200,10 +2200,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C16" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D16" t="s">
         <v>336</v>
@@ -2217,10 +2217,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D17" t="s">
         <v>336</v>
@@ -2234,10 +2234,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C18" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D18" t="s">
         <v>336</v>
@@ -2251,10 +2251,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>212</v>
+        <v>378</v>
       </c>
       <c r="C19" t="s">
-        <v>333</v>
+        <v>357</v>
       </c>
       <c r="E19" t="s">
         <v>215</v>
@@ -2367,10 +2367,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C26" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D26" t="s">
         <v>336</v>
@@ -2384,10 +2384,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C27" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D27" t="s">
         <v>336</v>
@@ -2928,7 +2928,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C59" t="s">
         <v>332</v>
@@ -2945,7 +2945,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C60" t="s">
         <v>332</v>
@@ -2962,7 +2962,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C61" t="s">
         <v>332</v>
@@ -2979,7 +2979,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C62" t="s">
         <v>332</v>
@@ -2996,7 +2996,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C63" t="s">
         <v>332</v>
@@ -3013,10 +3013,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>347</v>
+        <v>379</v>
       </c>
       <c r="C64" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="D64" t="s">
         <v>336</v>
@@ -3030,10 +3030,10 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>353</v>
+        <v>251</v>
       </c>
       <c r="C65" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="D65" t="s">
         <v>336</v>
@@ -3047,10 +3047,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>354</v>
+        <v>380</v>
       </c>
       <c r="C66" t="s">
-        <v>332</v>
+        <v>357</v>
       </c>
       <c r="D66" t="s">
         <v>336</v>
@@ -3268,7 +3268,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C79" t="s">
         <v>332</v>
@@ -3336,7 +3336,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C83" t="s">
         <v>332</v>
@@ -3353,7 +3353,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C84" t="s">
         <v>332</v>
@@ -3455,7 +3455,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C90" t="s">
         <v>332</v>
@@ -3489,7 +3489,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C92" t="s">
         <v>332</v>
@@ -4342,10 +4342,10 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C169" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D169" t="s">
         <v>336</v>
@@ -4359,10 +4359,10 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C170" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D170" t="s">
         <v>336</v>
@@ -4373,10 +4373,10 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C171" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D171" t="s">
         <v>336</v>
@@ -4387,10 +4387,10 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C172" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D172" t="s">
         <v>336</v>
@@ -4401,10 +4401,10 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C173" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D173" t="s">
         <v>336</v>
@@ -4415,10 +4415,10 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C174" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D174" t="s">
         <v>336</v>
@@ -4429,10 +4429,10 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C175" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D175" t="s">
         <v>336</v>
@@ -4443,10 +4443,10 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C176" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D176" t="s">
         <v>336</v>
@@ -4457,10 +4457,10 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C177" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D177" t="s">
         <v>336</v>
@@ -4471,10 +4471,10 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C178" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D178" t="s">
         <v>336</v>
@@ -4485,10 +4485,10 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C179" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D179" t="s">
         <v>336</v>
@@ -4499,10 +4499,10 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C180" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D180" t="s">
         <v>336</v>

</xml_diff>

<commit_message>
Added Scalability, Feature flags, Import products to catalog, Catalog publishing article
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C82F49B-1A19-4FA7-9663-F259890A9D19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF5B0BF-4F0D-4BF8-9027-EF890FD4313B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="381">
   <si>
     <t>Original Url</t>
   </si>
@@ -1066,12 +1066,6 @@
     <t>Create a new artilce /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module</t>
   </si>
   <si>
-    <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson1</t>
-  </si>
-  <si>
-    <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson2</t>
-  </si>
-  <si>
     <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson3</t>
   </si>
   <si>
@@ -1081,18 +1075,6 @@
     <t>/platform/developer-guide/Fundamentals/Indexed-Search/overview/</t>
   </si>
   <si>
-    <t>Copy content to platform/user-guide/catalog-publishing/overview/</t>
-  </si>
-  <si>
-    <t>Acomplish with the block for how to user groups propagation works platform/user-guide/catalog-personalization/overview/</t>
-  </si>
-  <si>
-    <t>copy content to platform/developer-guide/Tutorials-and-How-tos/override-rounding-policy</t>
-  </si>
-  <si>
-    <t>copy content to platform/user-guide/contacts/advanced-filter</t>
-  </si>
-  <si>
     <t>OnReview</t>
   </si>
   <si>
@@ -1163,6 +1145,24 @@
   </si>
   <si>
     <t>platform/developer-guide/Configuration-Reference/appsettingsjson/#__tabbed_2_2</t>
+  </si>
+  <si>
+    <t>platform/user-guide/marketing/dynamic-associations-overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/catalog-personalization/settings/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/catalog-publishing/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/contacts/filtering-options/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/overriding-rounding-policy/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/Tutorials/import-products-to-catalog/</t>
   </si>
 </sst>
 </file>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,10 +2149,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C13" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D13" t="s">
         <v>336</v>
@@ -2166,10 +2166,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C14" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D14" t="s">
         <v>336</v>
@@ -2183,10 +2183,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C15" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D15" t="s">
         <v>336</v>
@@ -2200,10 +2200,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C16" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D16" t="s">
         <v>336</v>
@@ -2217,10 +2217,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C17" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D17" t="s">
         <v>336</v>
@@ -2234,10 +2234,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C18" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D18" t="s">
         <v>336</v>
@@ -2251,10 +2251,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C19" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D19" t="s">
         <v>336</v>
@@ -2370,10 +2370,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C26" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D26" t="s">
         <v>336</v>
@@ -2387,10 +2387,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C27" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D27" t="s">
         <v>336</v>
@@ -2948,10 +2948,10 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>348</v>
+        <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="D60" t="s">
         <v>336</v>
@@ -2965,10 +2965,10 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>349</v>
+        <v>380</v>
       </c>
       <c r="C61" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="D61" t="s">
         <v>336</v>
@@ -2982,7 +2982,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C62" t="s">
         <v>332</v>
@@ -2999,7 +2999,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C63" t="s">
         <v>332</v>
@@ -3016,10 +3016,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C64" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D64" t="s">
         <v>336</v>
@@ -3036,7 +3036,7 @@
         <v>251</v>
       </c>
       <c r="C65" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D65" t="s">
         <v>336</v>
@@ -3050,10 +3050,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C66" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D66" t="s">
         <v>336</v>
@@ -3271,7 +3271,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C79" t="s">
         <v>332</v>
@@ -3339,10 +3339,10 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>354</v>
+        <v>376</v>
       </c>
       <c r="C83" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="D83" t="s">
         <v>336</v>
@@ -3356,10 +3356,10 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="C84" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="D84" t="s">
         <v>336</v>
@@ -3458,10 +3458,10 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="C90" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="D90" t="s">
         <v>336</v>
@@ -3492,10 +3492,10 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>356</v>
+        <v>378</v>
       </c>
       <c r="C92" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="D92" t="s">
         <v>336</v>
@@ -3548,7 +3548,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -3592,18 +3592,24 @@
         <v>332</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>279</v>
+        <v>375</v>
       </c>
       <c r="C101" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+      <c r="D101" t="s">
+        <v>336</v>
+      </c>
+      <c r="E101" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -3614,7 +3620,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -3625,7 +3631,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>104</v>
       </c>
@@ -3636,7 +3642,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>105</v>
       </c>
@@ -3647,7 +3653,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -3658,7 +3664,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -3669,7 +3675,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -3680,7 +3686,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -3691,7 +3697,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>110</v>
       </c>
@@ -3702,7 +3708,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -3713,7 +3719,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>112</v>
       </c>
@@ -4345,10 +4351,10 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C169" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D169" t="s">
         <v>336</v>
@@ -4362,10 +4368,10 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C170" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D170" t="s">
         <v>336</v>
@@ -4376,10 +4382,10 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C171" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D171" t="s">
         <v>336</v>
@@ -4390,10 +4396,10 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C172" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D172" t="s">
         <v>336</v>
@@ -4404,10 +4410,10 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C173" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D173" t="s">
         <v>336</v>
@@ -4418,10 +4424,10 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C174" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D174" t="s">
         <v>336</v>
@@ -4432,10 +4438,10 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C175" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D175" t="s">
         <v>336</v>
@@ -4446,10 +4452,10 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C176" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D176" t="s">
         <v>336</v>
@@ -4460,10 +4466,10 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C177" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D177" t="s">
         <v>336</v>
@@ -4474,10 +4480,10 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C178" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D178" t="s">
         <v>336</v>
@@ -4488,10 +4494,10 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C179" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D179" t="s">
         <v>336</v>
@@ -4502,10 +4508,10 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C180" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D180" t="s">
         <v>336</v>

</xml_diff>

<commit_message>
Order Manager role, Saved Credit cards articles
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F2F292-F846-45A8-BB1A-0001CB679A74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE5DAF2-1FC7-4336-B369-5B01CACD7D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="381">
   <si>
     <t>Original Url</t>
   </si>
@@ -2017,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3514,6 +3514,9 @@
       <c r="C93" t="s">
         <v>332</v>
       </c>
+      <c r="D93" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
@@ -3525,6 +3528,9 @@
       <c r="C94" t="s">
         <v>332</v>
       </c>
+      <c r="D94" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
@@ -3536,6 +3542,9 @@
       <c r="C95" t="s">
         <v>332</v>
       </c>
+      <c r="D95" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
@@ -3547,6 +3556,9 @@
       <c r="C96" t="s">
         <v>332</v>
       </c>
+      <c r="D96" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
@@ -3557,6 +3569,9 @@
       </c>
       <c r="C97" t="s">
         <v>332</v>
+      </c>
+      <c r="D97" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edge and Stable releases updates. Export/Import, CSV Import modules additions
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B132A997-0539-4656-A8D5-D556A2FE0E87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EB46D3-A953-48FD-B080-356A3E61F2E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="384">
   <si>
     <t>Original Url</t>
   </si>
@@ -2026,8 +2026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3526,6 +3526,9 @@
       <c r="D93" t="s">
         <v>337</v>
       </c>
+      <c r="E93" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
@@ -3540,6 +3543,9 @@
       <c r="D94" t="s">
         <v>337</v>
       </c>
+      <c r="E94" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
@@ -3554,6 +3560,9 @@
       <c r="D95" t="s">
         <v>337</v>
       </c>
+      <c r="E95" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
@@ -3568,6 +3577,9 @@
       <c r="D96" t="s">
         <v>337</v>
       </c>
+      <c r="E96" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
@@ -3582,6 +3594,9 @@
       <c r="D97" t="s">
         <v>337</v>
       </c>
+      <c r="E97" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
@@ -3596,6 +3611,9 @@
       <c r="D98" t="s">
         <v>336</v>
       </c>
+      <c r="E98" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -3610,6 +3628,9 @@
       <c r="D99" t="s">
         <v>336</v>
       </c>
+      <c r="E99" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
@@ -3621,6 +3642,12 @@
       <c r="C100" t="s">
         <v>332</v>
       </c>
+      <c r="D100" t="s">
+        <v>336</v>
+      </c>
+      <c r="E100" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
@@ -3652,6 +3679,9 @@
       <c r="D102" t="s">
         <v>336</v>
       </c>
+      <c r="E102" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
@@ -3751,6 +3781,12 @@
       <c r="C111" t="s">
         <v>332</v>
       </c>
+      <c r="D111" t="s">
+        <v>337</v>
+      </c>
+      <c r="E111" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
@@ -3762,8 +3798,14 @@
       <c r="C112" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>337</v>
+      </c>
+      <c r="E112" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -3773,8 +3815,14 @@
       <c r="C113" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>337</v>
+      </c>
+      <c r="E113" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>114</v>
       </c>
@@ -3784,8 +3832,14 @@
       <c r="C114" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>337</v>
+      </c>
+      <c r="E114" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -3795,8 +3849,14 @@
       <c r="C115" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>337</v>
+      </c>
+      <c r="E115" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>116</v>
       </c>
@@ -3807,7 +3867,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>117</v>
       </c>
@@ -3818,7 +3878,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>118</v>
       </c>
@@ -3829,7 +3889,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>119</v>
       </c>
@@ -3840,7 +3900,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>120</v>
       </c>
@@ -3851,7 +3911,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>121</v>
       </c>
@@ -3862,7 +3922,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>122</v>
       </c>
@@ -3873,7 +3933,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -3884,7 +3944,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>124</v>
       </c>
@@ -3895,7 +3955,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>125</v>
       </c>
@@ -3906,7 +3966,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>126</v>
       </c>
@@ -3917,7 +3977,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>127</v>
       </c>
@@ -3928,7 +3988,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
GDPR section added, CLI tools section updated
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0DEE76-D1A9-41CA-A951-FB6A46257E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D656BF89-4EEA-43A1-B4FE-496E70E64083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="387">
   <si>
     <t>Original Url</t>
   </si>
@@ -1069,9 +1069,6 @@
     <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson4</t>
   </si>
   <si>
-    <t>/platform/developer-guide/Fundamentals/Indexed-Search/overview/</t>
-  </si>
-  <si>
     <t>OnReview</t>
   </si>
   <si>
@@ -1175,6 +1172,15 @@
   </si>
   <si>
     <t>platform/user-guide/rating-reviews/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/gdpr/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/GraphQL-Storefront-API-Reference-xAPI/troubleshooting/</t>
+  </si>
+  <si>
+    <t>add new article</t>
   </si>
 </sst>
 </file>
@@ -2029,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,10 +2167,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D13" t="s">
         <v>336</v>
@@ -2178,10 +2184,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D14" t="s">
         <v>336</v>
@@ -2195,10 +2201,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D15" t="s">
         <v>336</v>
@@ -2212,10 +2218,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D16" t="s">
         <v>336</v>
@@ -2229,10 +2235,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D17" t="s">
         <v>336</v>
@@ -2246,10 +2252,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D18" t="s">
         <v>336</v>
@@ -2263,10 +2269,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D19" t="s">
         <v>336</v>
@@ -2382,10 +2388,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D26" t="s">
         <v>336</v>
@@ -2399,10 +2405,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D27" t="s">
         <v>336</v>
@@ -2535,10 +2541,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C35" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D35" t="s">
         <v>336</v>
@@ -2963,7 +2969,7 @@
         <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D60" t="s">
         <v>336</v>
@@ -2977,10 +2983,10 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C61" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D61" t="s">
         <v>336</v>
@@ -3028,10 +3034,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C64" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D64" t="s">
         <v>336</v>
@@ -3048,7 +3054,7 @@
         <v>251</v>
       </c>
       <c r="C65" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D65" t="s">
         <v>336</v>
@@ -3062,10 +3068,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C66" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D66" t="s">
         <v>336</v>
@@ -3283,7 +3289,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>349</v>
+        <v>226</v>
       </c>
       <c r="C79" t="s">
         <v>332</v>
@@ -3351,10 +3357,10 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C83" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D83" t="s">
         <v>336</v>
@@ -3368,10 +3374,10 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C84" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D84" t="s">
         <v>336</v>
@@ -3470,10 +3476,10 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C90" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D90" t="s">
         <v>336</v>
@@ -3504,10 +3510,10 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C92" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D92" t="s">
         <v>336</v>
@@ -3606,10 +3612,10 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C98" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D98" t="s">
         <v>336</v>
@@ -3623,10 +3629,10 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C99" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D99" t="s">
         <v>336</v>
@@ -3640,10 +3646,10 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C100" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D100" t="s">
         <v>336</v>
@@ -3657,10 +3663,10 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C101" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D101" t="s">
         <v>336</v>
@@ -3674,10 +3680,10 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C102" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D102" t="s">
         <v>336</v>
@@ -3740,16 +3746,28 @@
       <c r="C107" t="s">
         <v>332</v>
       </c>
+      <c r="D107" t="s">
+        <v>337</v>
+      </c>
+      <c r="E107" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>212</v>
+        <v>385</v>
       </c>
       <c r="C108" t="s">
         <v>332</v>
+      </c>
+      <c r="D108" t="s">
+        <v>337</v>
+      </c>
+      <c r="E108" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3762,6 +3780,12 @@
       <c r="C109" t="s">
         <v>332</v>
       </c>
+      <c r="D109" t="s">
+        <v>337</v>
+      </c>
+      <c r="E109" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
@@ -3872,6 +3896,12 @@
       <c r="C116" t="s">
         <v>332</v>
       </c>
+      <c r="D116" t="s">
+        <v>337</v>
+      </c>
+      <c r="E116" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
@@ -3883,16 +3913,28 @@
       <c r="C117" t="s">
         <v>332</v>
       </c>
+      <c r="D117" t="s">
+        <v>337</v>
+      </c>
+      <c r="E117" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>212</v>
+        <v>384</v>
       </c>
       <c r="C118" t="s">
-        <v>332</v>
+        <v>349</v>
+      </c>
+      <c r="D118" t="s">
+        <v>336</v>
+      </c>
+      <c r="E118" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3905,6 +3947,12 @@
       <c r="C119" t="s">
         <v>332</v>
       </c>
+      <c r="D119" t="s">
+        <v>337</v>
+      </c>
+      <c r="E119" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
@@ -3916,6 +3964,12 @@
       <c r="C120" t="s">
         <v>332</v>
       </c>
+      <c r="D120" t="s">
+        <v>337</v>
+      </c>
+      <c r="E120" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
@@ -3927,6 +3981,12 @@
       <c r="C121" t="s">
         <v>332</v>
       </c>
+      <c r="D121" t="s">
+        <v>337</v>
+      </c>
+      <c r="E121" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -3938,6 +3998,12 @@
       <c r="C122" t="s">
         <v>332</v>
       </c>
+      <c r="D122" t="s">
+        <v>337</v>
+      </c>
+      <c r="E122" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -3949,6 +4015,12 @@
       <c r="C123" t="s">
         <v>332</v>
       </c>
+      <c r="D123" t="s">
+        <v>337</v>
+      </c>
+      <c r="E123" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -3960,6 +4032,12 @@
       <c r="C124" t="s">
         <v>332</v>
       </c>
+      <c r="D124" t="s">
+        <v>337</v>
+      </c>
+      <c r="E124" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -3971,6 +4049,12 @@
       <c r="C125" t="s">
         <v>332</v>
       </c>
+      <c r="D125" t="s">
+        <v>337</v>
+      </c>
+      <c r="E125" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -3982,6 +4066,12 @@
       <c r="C126" t="s">
         <v>332</v>
       </c>
+      <c r="D126" t="s">
+        <v>337</v>
+      </c>
+      <c r="E126" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
@@ -3993,6 +4083,12 @@
       <c r="C127" t="s">
         <v>332</v>
       </c>
+      <c r="D127" t="s">
+        <v>337</v>
+      </c>
+      <c r="E127" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
@@ -4004,8 +4100,14 @@
       <c r="C128" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>337</v>
+      </c>
+      <c r="E128" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
@@ -4015,8 +4117,14 @@
       <c r="C129" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>337</v>
+      </c>
+      <c r="E129" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>130</v>
       </c>
@@ -4026,8 +4134,14 @@
       <c r="C130" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
+        <v>337</v>
+      </c>
+      <c r="E130" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>131</v>
       </c>
@@ -4037,8 +4151,14 @@
       <c r="C131" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>337</v>
+      </c>
+      <c r="E131" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>132</v>
       </c>
@@ -4048,8 +4168,11 @@
       <c r="C132" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>133</v>
       </c>
@@ -4059,8 +4182,14 @@
       <c r="C133" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>337</v>
+      </c>
+      <c r="E133" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>134</v>
       </c>
@@ -4070,8 +4199,11 @@
       <c r="C134" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>135</v>
       </c>
@@ -4081,8 +4213,14 @@
       <c r="C135" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>337</v>
+      </c>
+      <c r="E135" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>136</v>
       </c>
@@ -4092,8 +4230,14 @@
       <c r="C136" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>337</v>
+      </c>
+      <c r="E136" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>137</v>
       </c>
@@ -4103,8 +4247,14 @@
       <c r="C137" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>337</v>
+      </c>
+      <c r="E137" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>138</v>
       </c>
@@ -4114,8 +4264,14 @@
       <c r="C138" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
+        <v>337</v>
+      </c>
+      <c r="E138" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>139</v>
       </c>
@@ -4125,8 +4281,14 @@
       <c r="C139" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
+        <v>337</v>
+      </c>
+      <c r="E139" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>140</v>
       </c>
@@ -4136,8 +4298,14 @@
       <c r="C140" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
+        <v>337</v>
+      </c>
+      <c r="E140" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>141</v>
       </c>
@@ -4147,8 +4315,14 @@
       <c r="C141" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>337</v>
+      </c>
+      <c r="E141" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>142</v>
       </c>
@@ -4158,8 +4332,14 @@
       <c r="C142" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>337</v>
+      </c>
+      <c r="E142" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>143</v>
       </c>
@@ -4169,8 +4349,14 @@
       <c r="C143" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
+        <v>337</v>
+      </c>
+      <c r="E143" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>144</v>
       </c>
@@ -4180,19 +4366,31 @@
       <c r="C144" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>337</v>
+      </c>
+      <c r="E144" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>313</v>
+        <v>386</v>
       </c>
       <c r="C145" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>336</v>
+      </c>
+      <c r="E145" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>146</v>
       </c>
@@ -4202,8 +4400,14 @@
       <c r="C146" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
+        <v>337</v>
+      </c>
+      <c r="E146" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>147</v>
       </c>
@@ -4213,8 +4417,14 @@
       <c r="C147" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
+        <v>337</v>
+      </c>
+      <c r="E147" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>148</v>
       </c>
@@ -4224,8 +4434,14 @@
       <c r="C148" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
+        <v>337</v>
+      </c>
+      <c r="E148" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>149</v>
       </c>
@@ -4235,8 +4451,14 @@
       <c r="C149" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>337</v>
+      </c>
+      <c r="E149" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>150</v>
       </c>
@@ -4246,8 +4468,14 @@
       <c r="C150" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>337</v>
+      </c>
+      <c r="E150" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>151</v>
       </c>
@@ -4257,8 +4485,14 @@
       <c r="C151" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>337</v>
+      </c>
+      <c r="E151" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>152</v>
       </c>
@@ -4268,8 +4502,14 @@
       <c r="C152" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>337</v>
+      </c>
+      <c r="E152" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>153</v>
       </c>
@@ -4279,8 +4519,14 @@
       <c r="C153" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
+        <v>337</v>
+      </c>
+      <c r="E153" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>154</v>
       </c>
@@ -4290,8 +4536,14 @@
       <c r="C154" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
+        <v>337</v>
+      </c>
+      <c r="E154" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>155</v>
       </c>
@@ -4301,8 +4553,14 @@
       <c r="C155" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>337</v>
+      </c>
+      <c r="E155" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>156</v>
       </c>
@@ -4312,8 +4570,14 @@
       <c r="C156" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
+        <v>337</v>
+      </c>
+      <c r="E156" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>157</v>
       </c>
@@ -4323,8 +4587,14 @@
       <c r="C157" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>337</v>
+      </c>
+      <c r="E157" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>158</v>
       </c>
@@ -4334,8 +4604,11 @@
       <c r="C158" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>159</v>
       </c>
@@ -4346,7 +4619,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>160</v>
       </c>
@@ -4378,6 +4651,12 @@
       <c r="C162" t="s">
         <v>332</v>
       </c>
+      <c r="D162" t="s">
+        <v>337</v>
+      </c>
+      <c r="E162" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
@@ -4389,6 +4668,12 @@
       <c r="C163" t="s">
         <v>332</v>
       </c>
+      <c r="D163" t="s">
+        <v>337</v>
+      </c>
+      <c r="E163" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
@@ -4411,6 +4696,12 @@
       <c r="C165" t="s">
         <v>332</v>
       </c>
+      <c r="D165" t="s">
+        <v>337</v>
+      </c>
+      <c r="E165" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
@@ -4450,10 +4741,10 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C169" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D169" t="s">
         <v>336</v>
@@ -4467,10 +4758,10 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C170" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D170" t="s">
         <v>336</v>
@@ -4481,10 +4772,10 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C171" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D171" t="s">
         <v>336</v>
@@ -4495,10 +4786,10 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C172" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D172" t="s">
         <v>336</v>
@@ -4509,10 +4800,10 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C173" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D173" t="s">
         <v>336</v>
@@ -4523,10 +4814,10 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C174" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D174" t="s">
         <v>336</v>
@@ -4537,10 +4828,10 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C175" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D175" t="s">
         <v>336</v>
@@ -4551,10 +4842,10 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C176" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D176" t="s">
         <v>336</v>
@@ -4565,10 +4856,10 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C177" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D177" t="s">
         <v>336</v>
@@ -4579,10 +4870,10 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C178" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D178" t="s">
         <v>336</v>
@@ -4593,10 +4884,10 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C179" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D179" t="s">
         <v>336</v>
@@ -4607,10 +4898,10 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C180" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D180" t="s">
         <v>336</v>
@@ -4999,6 +5290,7 @@
     <hyperlink ref="A84" r:id="rId27" xr:uid="{4FBB0E83-5DCD-436A-94D0-3D97C5F74AA0}"/>
     <hyperlink ref="A90" r:id="rId28" xr:uid="{0B30FCB3-A6B1-481B-B95C-3C058F657A36}"/>
     <hyperlink ref="A92" r:id="rId29" xr:uid="{D4EA3FF3-9912-4F0B-BB5E-F0FD06FBC453}"/>
+    <hyperlink ref="A108" r:id="rId30" xr:uid="{05078AD5-984F-4FBF-AAF0-547BD01D0CF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
VC-build updates, Native payment method module description added
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D656BF89-4EEA-43A1-B4FE-496E70E64083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40850C7-3D96-4DC5-9D97-566BF6D1E86D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="388">
   <si>
     <t>Original Url</t>
   </si>
@@ -1181,6 +1181,9 @@
   </si>
   <si>
     <t>add new article</t>
+  </si>
+  <si>
+    <t>platform/user-guide/native-payment-methods/overview/</t>
   </si>
 </sst>
 </file>
@@ -2035,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3934,7 +3937,7 @@
         <v>336</v>
       </c>
       <c r="E118" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4190,17 +4193,20 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>212</v>
+        <v>387</v>
       </c>
       <c r="C134" t="s">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="D134" t="s">
         <v>336</v>
+      </c>
+      <c r="E134" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -5291,6 +5297,7 @@
     <hyperlink ref="A90" r:id="rId28" xr:uid="{0B30FCB3-A6B1-481B-B95C-3C058F657A36}"/>
     <hyperlink ref="A92" r:id="rId29" xr:uid="{D4EA3FF3-9912-4F0B-BB5E-F0FD06FBC453}"/>
     <hyperlink ref="A108" r:id="rId30" xr:uid="{05078AD5-984F-4FBF-AAF0-547BD01D0CF1}"/>
+    <hyperlink ref="A134" r:id="rId31" xr:uid="{16F8ED4E-A2AF-433A-BC67-2DB462120B1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CLI tools segment minor corrections
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40850C7-3D96-4DC5-9D97-566BF6D1E86D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3650AE-201A-4BEA-B23A-3BC854E9B49E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1075,9 +1075,6 @@
     <t>platform/developer-guide/CLI-tools/overview/</t>
   </si>
   <si>
-    <t>platform/developer-guide/CLI-tools/cold-start-data-migration/</t>
-  </si>
-  <si>
     <t>platform/developer-guide/CLI-tools/package-management/</t>
   </si>
   <si>
@@ -1184,6 +1181,9 @@
   </si>
   <si>
     <t>platform/user-guide/native-payment-methods/overview/</t>
+  </si>
+  <si>
+    <t>relocate article</t>
   </si>
 </sst>
 </file>
@@ -2039,7 +2039,7 @@
   <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2170,7 +2170,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C13" t="s">
         <v>349</v>
@@ -2187,10 +2187,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>351</v>
+        <v>387</v>
       </c>
       <c r="C14" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="D14" t="s">
         <v>336</v>
@@ -2204,7 +2204,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C15" t="s">
         <v>349</v>
@@ -2238,7 +2238,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C17" t="s">
         <v>349</v>
@@ -2255,7 +2255,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C18" t="s">
         <v>349</v>
@@ -2272,7 +2272,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C19" t="s">
         <v>349</v>
@@ -2391,7 +2391,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C26" t="s">
         <v>349</v>
@@ -2408,7 +2408,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C27" t="s">
         <v>349</v>
@@ -2544,7 +2544,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C35" t="s">
         <v>349</v>
@@ -2986,7 +2986,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C61" t="s">
         <v>349</v>
@@ -3037,7 +3037,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C64" t="s">
         <v>349</v>
@@ -3071,7 +3071,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C66" t="s">
         <v>349</v>
@@ -3360,7 +3360,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C83" t="s">
         <v>349</v>
@@ -3377,7 +3377,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C84" t="s">
         <v>349</v>
@@ -3479,7 +3479,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C90" t="s">
         <v>349</v>
@@ -3513,7 +3513,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C92" t="s">
         <v>349</v>
@@ -3615,7 +3615,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C98" t="s">
         <v>349</v>
@@ -3632,7 +3632,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C99" t="s">
         <v>349</v>
@@ -3649,7 +3649,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C100" t="s">
         <v>349</v>
@@ -3666,7 +3666,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C101" t="s">
         <v>349</v>
@@ -3683,7 +3683,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C102" t="s">
         <v>349</v>
@@ -3761,7 +3761,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C108" t="s">
         <v>332</v>
@@ -3928,7 +3928,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C118" t="s">
         <v>349</v>
@@ -4197,7 +4197,7 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C134" t="s">
         <v>349</v>
@@ -4384,7 +4384,7 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C145" t="s">
         <v>332</v>
@@ -4747,7 +4747,7 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C169" t="s">
         <v>349</v>
@@ -4764,7 +4764,7 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C170" t="s">
         <v>349</v>
@@ -4778,7 +4778,7 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C171" t="s">
         <v>349</v>
@@ -4792,7 +4792,7 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C172" t="s">
         <v>349</v>
@@ -4806,7 +4806,7 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C173" t="s">
         <v>349</v>
@@ -4820,7 +4820,7 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C174" t="s">
         <v>349</v>
@@ -4834,7 +4834,7 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C175" t="s">
         <v>349</v>
@@ -4848,7 +4848,7 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C176" t="s">
         <v>349</v>
@@ -4862,7 +4862,7 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C177" t="s">
         <v>349</v>
@@ -4876,7 +4876,7 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C178" t="s">
         <v>349</v>
@@ -4890,7 +4890,7 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C179" t="s">
         <v>349</v>
@@ -4904,7 +4904,7 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C180" t="s">
         <v>349</v>

</xml_diff>

<commit_message>
Added Push Messages module description, links to April Digest, Storefront and Platform sprint 6 updates
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3650AE-201A-4BEA-B23A-3BC854E9B49E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D24D84F-36DB-4128-AC44-56D8FC04B46B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="387">
   <si>
     <t>Original Url</t>
   </si>
@@ -766,9 +766,6 @@
     <t>https://virtocommerce.com/open-source-license</t>
   </si>
   <si>
-    <t>https://github.com/VirtoCommerce/vc-platform/releases</t>
-  </si>
-  <si>
     <t>https://www.virtocommerce.org/c/news-digest/</t>
   </si>
   <si>
@@ -1177,13 +1174,13 @@
     <t>platform/developer-guide/GraphQL-Storefront-API-Reference-xAPI/troubleshooting/</t>
   </si>
   <si>
-    <t>add new article</t>
-  </si>
-  <si>
     <t>platform/user-guide/native-payment-methods/overview/</t>
   </si>
   <si>
     <t>relocate article</t>
+  </si>
+  <si>
+    <t>platform/user-guide/payment/overview/</t>
   </si>
 </sst>
 </file>
@@ -2039,7 +2036,7 @@
   <dimension ref="A1:E211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C204" sqref="C204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,10 +2056,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E1" t="s">
         <v>214</v>
@@ -2076,7 +2073,7 @@
         <v>247</v>
       </c>
       <c r="C2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2087,7 +2084,7 @@
         <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2098,7 +2095,7 @@
         <v>219</v>
       </c>
       <c r="C4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2106,7 +2103,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2114,7 +2111,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2122,7 +2119,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2130,7 +2127,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,7 +2135,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2146,7 +2143,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2154,7 +2151,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2162,7 +2159,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,16 +2167,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2187,16 +2184,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2204,16 +2201,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,16 +2218,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2238,16 +2235,16 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2255,16 +2252,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2272,13 +2269,13 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E19" t="s">
         <v>215</v>
@@ -2289,16 +2286,16 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2306,16 +2303,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D21" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2323,16 +2320,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2340,16 +2337,16 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2357,16 +2354,16 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2377,13 +2374,13 @@
         <v>217</v>
       </c>
       <c r="C25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2391,16 +2388,16 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,16 +2405,16 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D27" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2428,13 +2425,13 @@
         <v>218</v>
       </c>
       <c r="C28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2445,13 +2442,13 @@
         <v>220</v>
       </c>
       <c r="C29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E29" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2462,13 +2459,13 @@
         <v>221</v>
       </c>
       <c r="C30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2479,13 +2476,13 @@
         <v>222</v>
       </c>
       <c r="C31" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E31" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2496,13 +2493,13 @@
         <v>223</v>
       </c>
       <c r="C32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E32" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2513,13 +2510,13 @@
         <v>224</v>
       </c>
       <c r="C33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2530,13 +2527,13 @@
         <v>225</v>
       </c>
       <c r="C34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2544,16 +2541,16 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C35" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D35" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2564,13 +2561,13 @@
         <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D36" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2581,13 +2578,13 @@
         <v>227</v>
       </c>
       <c r="C37" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E37" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2598,13 +2595,13 @@
         <v>228</v>
       </c>
       <c r="C38" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D38" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E38" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2615,13 +2612,13 @@
         <v>229</v>
       </c>
       <c r="C39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D39" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E39" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2632,13 +2629,13 @@
         <v>230</v>
       </c>
       <c r="C40" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E40" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2649,13 +2646,13 @@
         <v>231</v>
       </c>
       <c r="C41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,13 +2663,13 @@
         <v>232</v>
       </c>
       <c r="C42" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D42" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E42" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2683,13 +2680,13 @@
         <v>233</v>
       </c>
       <c r="C43" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D43" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E43" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2700,13 +2697,13 @@
         <v>234</v>
       </c>
       <c r="C44" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D44" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E44" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2717,13 +2714,13 @@
         <v>235</v>
       </c>
       <c r="C45" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D45" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E45" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2734,13 +2731,13 @@
         <v>236</v>
       </c>
       <c r="C46" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D46" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E46" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2751,13 +2748,13 @@
         <v>237</v>
       </c>
       <c r="C47" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D47" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E47" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2768,13 +2765,13 @@
         <v>238</v>
       </c>
       <c r="C48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E48" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2785,13 +2782,13 @@
         <v>239</v>
       </c>
       <c r="C49" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D49" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E49" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2802,13 +2799,13 @@
         <v>240</v>
       </c>
       <c r="C50" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D50" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E50" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2816,16 +2813,16 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C51" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D51" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E51" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2836,13 +2833,13 @@
         <v>241</v>
       </c>
       <c r="C52" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D52" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E52" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,13 +2850,13 @@
         <v>242</v>
       </c>
       <c r="C53" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D53" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2870,13 +2867,13 @@
         <v>243</v>
       </c>
       <c r="C54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D54" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E54" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2884,16 +2881,16 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C55" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D55" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E55" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2904,13 +2901,13 @@
         <v>244</v>
       </c>
       <c r="C56" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D56" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E56" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2921,13 +2918,13 @@
         <v>219</v>
       </c>
       <c r="C57" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D57" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E57" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2938,13 +2935,13 @@
         <v>245</v>
       </c>
       <c r="C58" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D58" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E58" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2952,16 +2949,16 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C59" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D59" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E59" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2972,13 +2969,13 @@
         <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D60" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E60" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2986,16 +2983,16 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C61" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D61" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E61" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3003,16 +3000,16 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C62" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D62" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E62" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3020,16 +3017,16 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C63" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D63" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E63" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3037,16 +3034,16 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C64" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D64" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3054,16 +3051,16 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C65" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D65" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E65" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3071,16 +3068,16 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C66" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D66" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E66" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3088,16 +3085,16 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C67" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D67" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E67" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3105,16 +3102,16 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D68" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E68" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3122,16 +3119,16 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C69" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D69" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E69" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3139,16 +3136,16 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C70" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D70" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E70" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3156,16 +3153,16 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C71" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D71" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E71" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3173,16 +3170,16 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C72" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D72" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E72" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3190,16 +3187,16 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C73" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D73" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E73" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3207,16 +3204,16 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C74" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D74" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E74" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3224,16 +3221,16 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C75" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D75" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E75" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3241,16 +3238,16 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C76" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D76" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E76" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,16 +3255,16 @@
         <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C77" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D77" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E77" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3275,16 +3272,16 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C78" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D78" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E78" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3295,13 +3292,13 @@
         <v>226</v>
       </c>
       <c r="C79" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D79" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E79" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3309,16 +3306,16 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C80" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E80" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3326,16 +3323,16 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C81" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D81" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E81" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3343,16 +3340,16 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C82" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D82" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E82" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3360,16 +3357,16 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D83" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E83" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3377,16 +3374,16 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C84" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D84" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E84" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3394,16 +3391,16 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C85" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D85" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E85" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3411,16 +3408,16 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C86" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D86" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E86" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3428,16 +3425,16 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C87" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D87" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E87" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3445,16 +3442,16 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C88" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D88" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E88" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3462,16 +3459,16 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C89" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D89" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E89" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3479,16 +3476,16 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C90" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D90" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E90" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3496,16 +3493,16 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C91" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D91" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E91" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3513,16 +3510,16 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C92" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D92" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E92" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3530,16 +3527,16 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C93" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D93" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E93" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3547,16 +3544,16 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C94" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D94" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E94" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3564,16 +3561,16 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C95" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D95" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E95" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,16 +3578,16 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C96" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D96" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E96" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3598,16 +3595,16 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C97" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D97" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E97" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3615,16 +3612,16 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C98" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D98" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E98" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3632,16 +3629,16 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C99" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D99" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E99" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3649,16 +3646,16 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C100" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D100" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E100" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3666,16 +3663,16 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C101" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D101" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E101" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3683,16 +3680,16 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C102" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D102" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E102" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3703,7 +3700,7 @@
         <v>212</v>
       </c>
       <c r="C103" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3714,7 +3711,7 @@
         <v>212</v>
       </c>
       <c r="C104" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3725,7 +3722,7 @@
         <v>212</v>
       </c>
       <c r="C105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3736,7 +3733,7 @@
         <v>212</v>
       </c>
       <c r="C106" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3744,16 +3741,16 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C107" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D107" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E107" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3761,16 +3758,16 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C108" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D108" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E108" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3778,16 +3775,16 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C109" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D109" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E109" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3795,13 +3792,13 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C110" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D110" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3809,16 +3806,16 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C111" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D111" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E111" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3826,16 +3823,16 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C112" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D112" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E112" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3843,16 +3840,16 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C113" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D113" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E113" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3860,16 +3857,16 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C114" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D114" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E114" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3877,16 +3874,16 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C115" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D115" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E115" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3894,16 +3891,16 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C116" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D116" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E116" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3911,16 +3908,16 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C117" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D117" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E117" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3928,16 +3925,16 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C118" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D118" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E118" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3945,16 +3942,16 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C119" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D119" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E119" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3962,16 +3959,16 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C120" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D120" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E120" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3979,16 +3976,16 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C121" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D121" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E121" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3996,16 +3993,16 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C122" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D122" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E122" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4013,16 +4010,16 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C123" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D123" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E123" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4030,16 +4027,16 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C124" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D124" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E124" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4047,16 +4044,16 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C125" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D125" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E125" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4064,16 +4061,16 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C126" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D126" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E126" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4081,16 +4078,16 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C127" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D127" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E127" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4098,16 +4095,16 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C128" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D128" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E128" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4115,16 +4112,16 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C129" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D129" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E129" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4132,16 +4129,16 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C130" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D130" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E130" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4149,16 +4146,16 @@
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C131" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D131" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E131" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4166,13 +4163,13 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C132" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D132" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4180,16 +4177,16 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C133" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D133" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E133" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4197,16 +4194,16 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C134" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D134" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E134" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,16 +4211,16 @@
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C135" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D135" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E135" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4231,16 +4228,16 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C136" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D136" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E136" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4248,16 +4245,16 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C137" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D137" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E137" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4265,16 +4262,16 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C138" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D138" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E138" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4282,16 +4279,16 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C139" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D139" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E139" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4299,16 +4296,16 @@
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C140" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D140" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E140" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4316,16 +4313,16 @@
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C141" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D141" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E141" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4333,16 +4330,16 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C142" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D142" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E142" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4350,16 +4347,16 @@
         <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C143" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D143" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E143" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4367,16 +4364,16 @@
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C144" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D144" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E144" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4384,16 +4381,16 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C145" t="s">
-        <v>332</v>
+        <v>348</v>
       </c>
       <c r="D145" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E145" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4401,16 +4398,16 @@
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C146" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D146" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E146" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4418,16 +4415,16 @@
         <v>147</v>
       </c>
       <c r="B147" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C147" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D147" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E147" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4435,16 +4432,16 @@
         <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C148" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D148" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E148" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4452,16 +4449,16 @@
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C149" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D149" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E149" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4469,16 +4466,16 @@
         <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C150" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D150" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E150" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4486,16 +4483,16 @@
         <v>151</v>
       </c>
       <c r="B151" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C151" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D151" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E151" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4503,16 +4500,16 @@
         <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C152" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D152" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E152" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4520,16 +4517,16 @@
         <v>153</v>
       </c>
       <c r="B153" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C153" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D153" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E153" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4537,16 +4534,16 @@
         <v>154</v>
       </c>
       <c r="B154" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C154" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D154" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E154" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4554,16 +4551,16 @@
         <v>155</v>
       </c>
       <c r="B155" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C155" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D155" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E155" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4571,16 +4568,16 @@
         <v>156</v>
       </c>
       <c r="B156" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C156" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D156" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E156" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4588,30 +4585,30 @@
         <v>157</v>
       </c>
       <c r="B157" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C157" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D157" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E157" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="A158" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B158" t="s">
         <v>212</v>
       </c>
       <c r="C158" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D158" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4619,10 +4616,13 @@
         <v>159</v>
       </c>
       <c r="B159" t="s">
-        <v>313</v>
+        <v>212</v>
       </c>
       <c r="C159" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D159" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4633,7 +4633,10 @@
         <v>212</v>
       </c>
       <c r="C160" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D160" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4641,10 +4644,16 @@
         <v>161</v>
       </c>
       <c r="B161" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C161" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D161" t="s">
+        <v>336</v>
+      </c>
+      <c r="E161" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4652,16 +4661,16 @@
         <v>162</v>
       </c>
       <c r="B162" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C162" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D162" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E162" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4669,16 +4678,16 @@
         <v>163</v>
       </c>
       <c r="B163" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C163" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D163" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E163" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4686,10 +4695,16 @@
         <v>164</v>
       </c>
       <c r="B164" t="s">
-        <v>212</v>
+        <v>312</v>
       </c>
       <c r="C164" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D164" t="s">
+        <v>336</v>
+      </c>
+      <c r="E164" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4697,16 +4712,16 @@
         <v>165</v>
       </c>
       <c r="B165" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C165" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D165" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E165" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -4717,7 +4732,10 @@
         <v>212</v>
       </c>
       <c r="C166" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D166" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4728,7 +4746,10 @@
         <v>212</v>
       </c>
       <c r="C167" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D167" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -4739,7 +4760,10 @@
         <v>212</v>
       </c>
       <c r="C168" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D168" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4747,16 +4771,16 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C169" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D169" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E169" t="s">
-        <v>248</v>
+        <v>343</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4764,13 +4788,16 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C170" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D170" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="E170" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4778,13 +4805,16 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C171" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D171" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="E171" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4792,13 +4822,16 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C172" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D172" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="E172" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4806,13 +4839,16 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C173" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D173" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="E173" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4820,13 +4856,16 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C174" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D174" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="E174" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4834,13 +4873,16 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C175" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D175" t="s">
-        <v>336</v>
+        <v>335</v>
+      </c>
+      <c r="E175" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4848,83 +4890,104 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C176" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D176" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="E176" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C177" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D177" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="E177" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C178" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D178" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="E178" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C179" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D179" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="E179" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C180" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D180" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="E180" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>181</v>
       </c>
       <c r="B181" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C181" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="D181" t="s">
+        <v>335</v>
+      </c>
+      <c r="E181" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>182</v>
       </c>
@@ -4932,10 +4995,10 @@
         <v>216</v>
       </c>
       <c r="C182" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>183</v>
       </c>
@@ -4943,10 +5006,10 @@
         <v>216</v>
       </c>
       <c r="C183" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>184</v>
       </c>
@@ -4954,10 +5017,10 @@
         <v>216</v>
       </c>
       <c r="C184" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>185</v>
       </c>
@@ -4965,10 +5028,10 @@
         <v>216</v>
       </c>
       <c r="C185" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>186</v>
       </c>
@@ -4976,10 +5039,10 @@
         <v>216</v>
       </c>
       <c r="C186" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>187</v>
       </c>
@@ -4987,10 +5050,10 @@
         <v>216</v>
       </c>
       <c r="C187" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>188</v>
       </c>
@@ -4998,32 +5061,44 @@
         <v>216</v>
       </c>
       <c r="C188" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>189</v>
       </c>
       <c r="B189" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C189" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="D189" t="s">
+        <v>335</v>
+      </c>
+      <c r="E189" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>190</v>
       </c>
       <c r="B190" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C190" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="D190" t="s">
+        <v>335</v>
+      </c>
+      <c r="E190" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>191</v>
       </c>
@@ -5031,18 +5106,27 @@
         <v>212</v>
       </c>
       <c r="C191" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+      <c r="D191" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>192</v>
       </c>
       <c r="B192" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C192" t="s">
-        <v>332</v>
+        <v>348</v>
+      </c>
+      <c r="D192" t="s">
+        <v>335</v>
+      </c>
+      <c r="E192" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5053,7 +5137,10 @@
         <v>212</v>
       </c>
       <c r="C193" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D193" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5064,7 +5151,10 @@
         <v>212</v>
       </c>
       <c r="C194" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D194" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -5075,7 +5165,10 @@
         <v>212</v>
       </c>
       <c r="C195" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D195" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5086,7 +5179,10 @@
         <v>212</v>
       </c>
       <c r="C196" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D196" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -5097,7 +5193,10 @@
         <v>212</v>
       </c>
       <c r="C197" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D197" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5105,10 +5204,16 @@
         <v>198</v>
       </c>
       <c r="B198" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C198" t="s">
-        <v>332</v>
+        <v>348</v>
+      </c>
+      <c r="D198" t="s">
+        <v>335</v>
+      </c>
+      <c r="E198" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5119,7 +5224,10 @@
         <v>212</v>
       </c>
       <c r="C199" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D199" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5130,7 +5238,10 @@
         <v>212</v>
       </c>
       <c r="C200" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D200" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5141,7 +5252,10 @@
         <v>212</v>
       </c>
       <c r="C201" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D201" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5152,7 +5266,10 @@
         <v>212</v>
       </c>
       <c r="C202" t="s">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="D202" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5160,10 +5277,16 @@
         <v>203</v>
       </c>
       <c r="B203" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C203" t="s">
-        <v>332</v>
+        <v>348</v>
+      </c>
+      <c r="D203" t="s">
+        <v>335</v>
+      </c>
+      <c r="E203" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5171,10 +5294,10 @@
         <v>204</v>
       </c>
       <c r="B204" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C204" t="s">
-        <v>332</v>
+        <v>348</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5182,10 +5305,10 @@
         <v>205</v>
       </c>
       <c r="B205" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C205" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5193,10 +5316,10 @@
         <v>206</v>
       </c>
       <c r="B206" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C206" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5204,10 +5327,10 @@
         <v>207</v>
       </c>
       <c r="B207" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C207" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5218,10 +5341,10 @@
         <v>246</v>
       </c>
       <c r="C208" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E208" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -5232,7 +5355,7 @@
         <v>212</v>
       </c>
       <c r="C209" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -5240,10 +5363,10 @@
         <v>210</v>
       </c>
       <c r="B210" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C210" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -5251,10 +5374,10 @@
         <v>211</v>
       </c>
       <c r="B211" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C211" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -5271,33 +5394,33 @@
     <hyperlink ref="A13" r:id="rId2" xr:uid="{1C549BF6-83D2-4C75-AE1D-C2F86A653D1A}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{2F778272-CD26-4C05-A595-DF14512CE623}"/>
     <hyperlink ref="E27" r:id="rId4" display="https://virtostart-demo-admin.govirto.com/docs/index.html" xr:uid="{2F69C9CC-1055-414D-9C75-56CCCD337F48}"/>
-    <hyperlink ref="E169" r:id="rId5" xr:uid="{C639680D-E96B-460A-B8F9-109863FB0F34}"/>
-    <hyperlink ref="A18" r:id="rId6" xr:uid="{3EE074AE-E7B4-410B-995E-14E385EBD9D9}"/>
-    <hyperlink ref="A20" r:id="rId7" xr:uid="{A846E1E7-1C10-438C-8D77-B29FB7B9DDCB}"/>
-    <hyperlink ref="B20" r:id="rId8" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/Tutorials/creating-custom-module/" xr:uid="{20723581-A5B8-40ED-9B17-3E77BBDED0EE}"/>
-    <hyperlink ref="A21" r:id="rId9" xr:uid="{13623968-93F4-4187-901B-4CBAB89D76F0}"/>
-    <hyperlink ref="B21" r:id="rId10" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/" xr:uid="{E30A31FF-1C73-4CA9-A021-B80BED4646E7}"/>
-    <hyperlink ref="A22" r:id="rId11" xr:uid="{0E681307-BB1C-4BD8-8A9E-5044EC1C59B6}"/>
-    <hyperlink ref="B22" r:id="rId12" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/" xr:uid="{AA700B5F-11D7-4E1E-9611-FE738BEF6BC4}"/>
-    <hyperlink ref="A23" r:id="rId13" xr:uid="{D676FAF4-1680-4AE0-B48E-4C1F894CC542}"/>
-    <hyperlink ref="A24" r:id="rId14" xr:uid="{51CA47E3-9EDA-4F3F-9A20-DA44C4B36016}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{EBD2BA40-D76F-4105-B6BA-313C8046E566}"/>
-    <hyperlink ref="A26" r:id="rId16" xr:uid="{736CF484-2649-4C60-BDBD-AA3027BC4179}"/>
-    <hyperlink ref="A27" r:id="rId17" xr:uid="{7BD62CB9-4B34-45EF-911B-C961E0490377}"/>
-    <hyperlink ref="A28" r:id="rId18" xr:uid="{A76A15B9-FDDE-49A2-9A79-B78E65D68304}"/>
-    <hyperlink ref="A35" r:id="rId19" xr:uid="{7FE9D0BF-2813-442F-9B0A-E1D382D595B0}"/>
-    <hyperlink ref="A51" r:id="rId20" xr:uid="{B085393A-1208-4897-8C53-B853C7A540DA}"/>
-    <hyperlink ref="A59" r:id="rId21" xr:uid="{C9E5A96B-07CA-4609-B494-FFD7139FF80F}"/>
-    <hyperlink ref="A64" r:id="rId22" xr:uid="{0D02B00C-8889-41AD-A5C7-868F266E5D07}"/>
-    <hyperlink ref="A60" r:id="rId23" xr:uid="{728667AF-BEB9-41A4-A80B-FBD8B37A60E0}"/>
-    <hyperlink ref="A65" r:id="rId24" xr:uid="{E5E95940-AF1C-4DD9-A0B1-14074CE6C427}"/>
-    <hyperlink ref="A66" r:id="rId25" xr:uid="{1C5554FC-04EC-47BC-89DB-1728DBAE98CB}"/>
-    <hyperlink ref="A79" r:id="rId26" xr:uid="{D8CF9C4B-F15C-4E37-AA00-9F1BFEA56A7E}"/>
-    <hyperlink ref="A84" r:id="rId27" xr:uid="{4FBB0E83-5DCD-436A-94D0-3D97C5F74AA0}"/>
-    <hyperlink ref="A90" r:id="rId28" xr:uid="{0B30FCB3-A6B1-481B-B95C-3C058F657A36}"/>
-    <hyperlink ref="A92" r:id="rId29" xr:uid="{D4EA3FF3-9912-4F0B-BB5E-F0FD06FBC453}"/>
-    <hyperlink ref="A108" r:id="rId30" xr:uid="{05078AD5-984F-4FBF-AAF0-547BD01D0CF1}"/>
-    <hyperlink ref="A134" r:id="rId31" xr:uid="{16F8ED4E-A2AF-433A-BC67-2DB462120B1B}"/>
+    <hyperlink ref="A18" r:id="rId5" xr:uid="{3EE074AE-E7B4-410B-995E-14E385EBD9D9}"/>
+    <hyperlink ref="A20" r:id="rId6" xr:uid="{A846E1E7-1C10-438C-8D77-B29FB7B9DDCB}"/>
+    <hyperlink ref="B20" r:id="rId7" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/Tutorials/creating-custom-module/" xr:uid="{20723581-A5B8-40ED-9B17-3E77BBDED0EE}"/>
+    <hyperlink ref="A21" r:id="rId8" xr:uid="{13623968-93F4-4187-901B-4CBAB89D76F0}"/>
+    <hyperlink ref="B21" r:id="rId9" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/" xr:uid="{E30A31FF-1C73-4CA9-A021-B80BED4646E7}"/>
+    <hyperlink ref="A22" r:id="rId10" xr:uid="{0E681307-BB1C-4BD8-8A9E-5044EC1C59B6}"/>
+    <hyperlink ref="B22" r:id="rId11" display="https://docs.virtocommerce.org/platform/developer-guide/Tutorials-and-How-tos/How-tos/debugging/" xr:uid="{AA700B5F-11D7-4E1E-9611-FE738BEF6BC4}"/>
+    <hyperlink ref="A23" r:id="rId12" xr:uid="{D676FAF4-1680-4AE0-B48E-4C1F894CC542}"/>
+    <hyperlink ref="A24" r:id="rId13" xr:uid="{51CA47E3-9EDA-4F3F-9A20-DA44C4B36016}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{EBD2BA40-D76F-4105-B6BA-313C8046E566}"/>
+    <hyperlink ref="A26" r:id="rId15" xr:uid="{736CF484-2649-4C60-BDBD-AA3027BC4179}"/>
+    <hyperlink ref="A27" r:id="rId16" xr:uid="{7BD62CB9-4B34-45EF-911B-C961E0490377}"/>
+    <hyperlink ref="A28" r:id="rId17" xr:uid="{A76A15B9-FDDE-49A2-9A79-B78E65D68304}"/>
+    <hyperlink ref="A35" r:id="rId18" xr:uid="{7FE9D0BF-2813-442F-9B0A-E1D382D595B0}"/>
+    <hyperlink ref="A51" r:id="rId19" xr:uid="{B085393A-1208-4897-8C53-B853C7A540DA}"/>
+    <hyperlink ref="A59" r:id="rId20" xr:uid="{C9E5A96B-07CA-4609-B494-FFD7139FF80F}"/>
+    <hyperlink ref="A64" r:id="rId21" xr:uid="{0D02B00C-8889-41AD-A5C7-868F266E5D07}"/>
+    <hyperlink ref="A60" r:id="rId22" xr:uid="{728667AF-BEB9-41A4-A80B-FBD8B37A60E0}"/>
+    <hyperlink ref="A65" r:id="rId23" xr:uid="{E5E95940-AF1C-4DD9-A0B1-14074CE6C427}"/>
+    <hyperlink ref="A66" r:id="rId24" xr:uid="{1C5554FC-04EC-47BC-89DB-1728DBAE98CB}"/>
+    <hyperlink ref="A79" r:id="rId25" xr:uid="{D8CF9C4B-F15C-4E37-AA00-9F1BFEA56A7E}"/>
+    <hyperlink ref="A84" r:id="rId26" xr:uid="{4FBB0E83-5DCD-436A-94D0-3D97C5F74AA0}"/>
+    <hyperlink ref="A90" r:id="rId27" xr:uid="{0B30FCB3-A6B1-481B-B95C-3C058F657A36}"/>
+    <hyperlink ref="A92" r:id="rId28" xr:uid="{D4EA3FF3-9912-4F0B-BB5E-F0FD06FBC453}"/>
+    <hyperlink ref="A108" r:id="rId29" xr:uid="{05078AD5-984F-4FBF-AAF0-547BD01D0CF1}"/>
+    <hyperlink ref="A134" r:id="rId30" xr:uid="{16F8ED4E-A2AF-433A-BC67-2DB462120B1B}"/>
+    <hyperlink ref="A158" r:id="rId31" xr:uid="{27210CD7-8CAB-47C6-B488-A8E7B95F5B2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Search module description and corrected appsettings.json
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D24D84F-36DB-4128-AC44-56D8FC04B46B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF9072-1B21-4D8F-B855-EC9DC9B954BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1177,10 +1177,10 @@
     <t>platform/user-guide/native-payment-methods/overview/</t>
   </si>
   <si>
-    <t>relocate article</t>
-  </si>
-  <si>
     <t>platform/user-guide/payment/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/CLI-tools/cold-start-data-migration/</t>
   </si>
 </sst>
 </file>
@@ -2035,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C204" sqref="C204"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,10 +2184,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C14" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
       <c r="D14" t="s">
         <v>335</v>
@@ -3693,7 +3693,7 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B103" t="s">
@@ -4381,7 +4381,7 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C145" t="s">
         <v>348</v>
@@ -5421,6 +5421,7 @@
     <hyperlink ref="A108" r:id="rId29" xr:uid="{05078AD5-984F-4FBF-AAF0-547BD01D0CF1}"/>
     <hyperlink ref="A134" r:id="rId30" xr:uid="{16F8ED4E-A2AF-433A-BC67-2DB462120B1B}"/>
     <hyperlink ref="A158" r:id="rId31" xr:uid="{27210CD7-8CAB-47C6-B488-A8E7B95F5B2C}"/>
+    <hyperlink ref="A103" r:id="rId32" xr:uid="{9B568E95-26EE-4D47-B494-E1484996E56D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Search engines modules added and updated, scalability article updated
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF9072-1B21-4D8F-B855-EC9DC9B954BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5C2B4-B813-413E-AD06-29E405C58298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="390">
   <si>
     <t>Original Url</t>
   </si>
@@ -1009,9 +1009,6 @@
     <t>github.com/VirtoCommerce/vc-platform/tree/dev/docs/products</t>
   </si>
   <si>
-    <t>platform/user-guide/cart/settings/</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -1181,6 +1178,18 @@
   </si>
   <si>
     <t>platform/developer-guide/CLI-tools/cold-start-data-migration/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/cart/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/search/managing-search/#blue-green-indexing</t>
+  </si>
+  <si>
+    <t>platform/user-guide/elastic-search/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/elastic-app-search/overview/</t>
   </si>
 </sst>
 </file>
@@ -1331,7 +1340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1511,6 +1520,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1673,10 +1688,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2035,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,10 +2074,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E1" t="s">
         <v>214</v>
@@ -2073,7 +2091,7 @@
         <v>247</v>
       </c>
       <c r="C2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2084,7 +2102,7 @@
         <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2095,7 +2113,7 @@
         <v>219</v>
       </c>
       <c r="C4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2103,7 +2121,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2111,7 +2129,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2119,7 +2137,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2127,7 +2145,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2135,7 +2153,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2143,7 +2161,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2151,7 +2169,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2159,7 +2177,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2167,16 +2185,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2184,16 +2202,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2201,16 +2219,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2218,16 +2236,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2235,16 +2253,16 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2252,16 +2270,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D18" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E18" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2269,13 +2287,13 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E19" t="s">
         <v>215</v>
@@ -2286,16 +2304,16 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2303,16 +2321,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D21" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2320,16 +2338,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D22" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2337,16 +2355,16 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D23" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,16 +2372,16 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C24" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D24" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,13 +2392,13 @@
         <v>217</v>
       </c>
       <c r="C25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2388,16 +2406,16 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2405,16 +2423,16 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D27" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2425,13 +2443,13 @@
         <v>218</v>
       </c>
       <c r="C28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,13 +2460,13 @@
         <v>220</v>
       </c>
       <c r="C29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2459,13 +2477,13 @@
         <v>221</v>
       </c>
       <c r="C30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2476,13 +2494,13 @@
         <v>222</v>
       </c>
       <c r="C31" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D31" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E31" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2493,13 +2511,13 @@
         <v>223</v>
       </c>
       <c r="C32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E32" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2510,13 +2528,13 @@
         <v>224</v>
       </c>
       <c r="C33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2527,13 +2545,13 @@
         <v>225</v>
       </c>
       <c r="C34" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2541,16 +2559,16 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C35" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E35" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2561,13 +2579,13 @@
         <v>226</v>
       </c>
       <c r="C36" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E36" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,13 +2596,13 @@
         <v>227</v>
       </c>
       <c r="C37" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2595,13 +2613,13 @@
         <v>228</v>
       </c>
       <c r="C38" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D38" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E38" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,13 +2630,13 @@
         <v>229</v>
       </c>
       <c r="C39" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E39" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2629,13 +2647,13 @@
         <v>230</v>
       </c>
       <c r="C40" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2646,13 +2664,13 @@
         <v>231</v>
       </c>
       <c r="C41" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2663,13 +2681,13 @@
         <v>232</v>
       </c>
       <c r="C42" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D42" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E42" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,13 +2698,13 @@
         <v>233</v>
       </c>
       <c r="C43" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D43" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E43" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2697,13 +2715,13 @@
         <v>234</v>
       </c>
       <c r="C44" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E44" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,13 +2732,13 @@
         <v>235</v>
       </c>
       <c r="C45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E45" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2731,13 +2749,13 @@
         <v>236</v>
       </c>
       <c r="C46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E46" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2748,13 +2766,13 @@
         <v>237</v>
       </c>
       <c r="C47" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E47" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2765,13 +2783,13 @@
         <v>238</v>
       </c>
       <c r="C48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2782,13 +2800,13 @@
         <v>239</v>
       </c>
       <c r="C49" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D49" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E49" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2799,13 +2817,13 @@
         <v>240</v>
       </c>
       <c r="C50" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D50" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E50" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2813,16 +2831,16 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C51" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D51" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E51" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2833,13 +2851,13 @@
         <v>241</v>
       </c>
       <c r="C52" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D52" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E52" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2850,13 +2868,13 @@
         <v>242</v>
       </c>
       <c r="C53" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D53" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E53" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2867,13 +2885,13 @@
         <v>243</v>
       </c>
       <c r="C54" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D54" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E54" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2884,13 +2902,13 @@
         <v>327</v>
       </c>
       <c r="C55" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D55" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E55" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2901,13 +2919,13 @@
         <v>244</v>
       </c>
       <c r="C56" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D56" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E56" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2918,13 +2936,13 @@
         <v>219</v>
       </c>
       <c r="C57" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D57" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E57" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,30 +2953,30 @@
         <v>245</v>
       </c>
       <c r="C58" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D58" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E58" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B59" t="s">
-        <v>345</v>
-      </c>
-      <c r="C59" t="s">
-        <v>331</v>
-      </c>
-      <c r="D59" t="s">
-        <v>335</v>
-      </c>
-      <c r="E59" t="s">
-        <v>343</v>
+      <c r="B59" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2969,13 +2987,13 @@
         <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D60" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E60" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2983,50 +3001,50 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D61" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E61" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="C62" t="s">
-        <v>331</v>
-      </c>
-      <c r="D62" t="s">
-        <v>335</v>
-      </c>
-      <c r="E62" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" t="s">
-        <v>347</v>
-      </c>
-      <c r="C63" t="s">
-        <v>331</v>
-      </c>
-      <c r="D63" t="s">
-        <v>335</v>
-      </c>
-      <c r="E63" t="s">
-        <v>343</v>
+      <c r="C63" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3034,16 +3052,16 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C64" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D64" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E64" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3054,13 +3072,13 @@
         <v>250</v>
       </c>
       <c r="C65" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D65" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E65" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3068,16 +3086,16 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C66" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D66" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E66" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3085,16 +3103,16 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>329</v>
+        <v>386</v>
       </c>
       <c r="C67" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D67" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E67" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3105,13 +3123,13 @@
         <v>258</v>
       </c>
       <c r="C68" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D68" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E68" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3122,13 +3140,13 @@
         <v>259</v>
       </c>
       <c r="C69" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D69" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E69" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3139,13 +3157,13 @@
         <v>260</v>
       </c>
       <c r="C70" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D70" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E70" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3156,13 +3174,13 @@
         <v>261</v>
       </c>
       <c r="C71" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D71" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E71" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3173,13 +3191,13 @@
         <v>261</v>
       </c>
       <c r="C72" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E72" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3190,13 +3208,13 @@
         <v>262</v>
       </c>
       <c r="C73" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D73" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E73" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3207,13 +3225,13 @@
         <v>263</v>
       </c>
       <c r="C74" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D74" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E74" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3224,13 +3242,13 @@
         <v>264</v>
       </c>
       <c r="C75" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E75" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3241,13 +3259,13 @@
         <v>265</v>
       </c>
       <c r="C76" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D76" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E76" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,13 +3276,13 @@
         <v>266</v>
       </c>
       <c r="C77" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D77" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E77" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3275,13 +3293,13 @@
         <v>267</v>
       </c>
       <c r="C78" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D78" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E78" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3292,13 +3310,13 @@
         <v>226</v>
       </c>
       <c r="C79" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D79" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E79" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3309,13 +3327,13 @@
         <v>268</v>
       </c>
       <c r="C80" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D80" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3326,13 +3344,13 @@
         <v>269</v>
       </c>
       <c r="C81" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D81" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E81" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3343,13 +3361,13 @@
         <v>270</v>
       </c>
       <c r="C82" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D82" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E82" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3357,16 +3375,16 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C83" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D83" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E83" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3374,16 +3392,16 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D84" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E84" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3394,13 +3412,13 @@
         <v>271</v>
       </c>
       <c r="C85" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D85" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E85" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3411,13 +3429,13 @@
         <v>272</v>
       </c>
       <c r="C86" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D86" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E86" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3428,13 +3446,13 @@
         <v>273</v>
       </c>
       <c r="C87" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D87" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E87" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3445,13 +3463,13 @@
         <v>274</v>
       </c>
       <c r="C88" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D88" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E88" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3462,13 +3480,13 @@
         <v>275</v>
       </c>
       <c r="C89" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D89" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E89" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3476,16 +3494,16 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C90" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D90" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E90" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3496,13 +3514,13 @@
         <v>276</v>
       </c>
       <c r="C91" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D91" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E91" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3510,16 +3528,16 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C92" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D92" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E92" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3530,13 +3548,13 @@
         <v>277</v>
       </c>
       <c r="C93" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D93" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E93" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3547,13 +3565,13 @@
         <v>277</v>
       </c>
       <c r="C94" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D94" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E94" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3564,13 +3582,13 @@
         <v>277</v>
       </c>
       <c r="C95" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D95" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E95" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,13 +3599,13 @@
         <v>277</v>
       </c>
       <c r="C96" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D96" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E96" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3598,13 +3616,13 @@
         <v>277</v>
       </c>
       <c r="C97" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D97" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E97" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3612,16 +3630,16 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C98" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D98" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E98" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3629,16 +3647,16 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C99" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D99" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E99" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3646,16 +3664,16 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C100" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D100" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E100" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3663,16 +3681,16 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C101" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D101" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E101" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3680,16 +3698,16 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C102" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D102" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E102" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3697,10 +3715,16 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>212</v>
+        <v>389</v>
       </c>
       <c r="C103" t="s">
-        <v>331</v>
+        <v>347</v>
+      </c>
+      <c r="D103" t="s">
+        <v>334</v>
+      </c>
+      <c r="E103" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3708,10 +3732,16 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>212</v>
+        <v>388</v>
       </c>
       <c r="C104" t="s">
-        <v>331</v>
+        <v>347</v>
+      </c>
+      <c r="D104" t="s">
+        <v>334</v>
+      </c>
+      <c r="E104" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3719,10 +3749,16 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>212</v>
+        <v>387</v>
       </c>
       <c r="C105" t="s">
-        <v>331</v>
+        <v>347</v>
+      </c>
+      <c r="D105" t="s">
+        <v>334</v>
+      </c>
+      <c r="E105" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3733,7 +3769,7 @@
         <v>212</v>
       </c>
       <c r="C106" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3744,13 +3780,13 @@
         <v>279</v>
       </c>
       <c r="C107" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D107" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E107" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3758,16 +3794,16 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C108" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D108" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E108" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3778,13 +3814,13 @@
         <v>281</v>
       </c>
       <c r="C109" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D109" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E109" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3795,10 +3831,10 @@
         <v>282</v>
       </c>
       <c r="C110" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D110" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3809,13 +3845,13 @@
         <v>280</v>
       </c>
       <c r="C111" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D111" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E111" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3826,13 +3862,13 @@
         <v>283</v>
       </c>
       <c r="C112" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D112" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E112" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3843,13 +3879,13 @@
         <v>284</v>
       </c>
       <c r="C113" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D113" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E113" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3860,13 +3896,13 @@
         <v>285</v>
       </c>
       <c r="C114" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D114" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E114" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3877,13 +3913,13 @@
         <v>286</v>
       </c>
       <c r="C115" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D115" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E115" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3894,13 +3930,13 @@
         <v>287</v>
       </c>
       <c r="C116" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E116" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3911,13 +3947,13 @@
         <v>288</v>
       </c>
       <c r="C117" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D117" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E117" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3925,16 +3961,16 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C118" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D118" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E118" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3945,13 +3981,13 @@
         <v>289</v>
       </c>
       <c r="C119" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D119" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E119" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3962,13 +3998,13 @@
         <v>290</v>
       </c>
       <c r="C120" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D120" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E120" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3979,13 +4015,13 @@
         <v>291</v>
       </c>
       <c r="C121" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D121" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E121" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3996,13 +4032,13 @@
         <v>292</v>
       </c>
       <c r="C122" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D122" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E122" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4013,13 +4049,13 @@
         <v>293</v>
       </c>
       <c r="C123" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D123" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E123" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4030,13 +4066,13 @@
         <v>278</v>
       </c>
       <c r="C124" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D124" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E124" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4047,13 +4083,13 @@
         <v>294</v>
       </c>
       <c r="C125" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D125" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E125" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4064,13 +4100,13 @@
         <v>295</v>
       </c>
       <c r="C126" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D126" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E126" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4081,13 +4117,13 @@
         <v>296</v>
       </c>
       <c r="C127" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D127" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E127" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4098,13 +4134,13 @@
         <v>297</v>
       </c>
       <c r="C128" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D128" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E128" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4115,13 +4151,13 @@
         <v>298</v>
       </c>
       <c r="C129" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D129" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E129" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4132,13 +4168,13 @@
         <v>299</v>
       </c>
       <c r="C130" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D130" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E130" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4149,13 +4185,13 @@
         <v>300</v>
       </c>
       <c r="C131" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D131" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E131" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4166,10 +4202,10 @@
         <v>301</v>
       </c>
       <c r="C132" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D132" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4180,13 +4216,13 @@
         <v>302</v>
       </c>
       <c r="C133" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D133" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E133" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4194,16 +4230,16 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C134" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D134" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E134" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,13 +4250,13 @@
         <v>303</v>
       </c>
       <c r="C135" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D135" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E135" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4231,13 +4267,13 @@
         <v>304</v>
       </c>
       <c r="C136" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D136" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E136" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4248,13 +4284,13 @@
         <v>305</v>
       </c>
       <c r="C137" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D137" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E137" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4265,13 +4301,13 @@
         <v>306</v>
       </c>
       <c r="C138" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D138" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E138" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4282,13 +4318,13 @@
         <v>307</v>
       </c>
       <c r="C139" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D139" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E139" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4299,13 +4335,13 @@
         <v>308</v>
       </c>
       <c r="C140" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D140" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E140" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4316,13 +4352,13 @@
         <v>309</v>
       </c>
       <c r="C141" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D141" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E141" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4333,13 +4369,13 @@
         <v>310</v>
       </c>
       <c r="C142" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D142" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E142" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4350,13 +4386,13 @@
         <v>308</v>
       </c>
       <c r="C143" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D143" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E143" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4367,13 +4403,13 @@
         <v>311</v>
       </c>
       <c r="C144" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D144" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E144" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4381,16 +4417,16 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C145" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D145" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E145" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4401,13 +4437,13 @@
         <v>313</v>
       </c>
       <c r="C146" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D146" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E146" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4418,13 +4454,13 @@
         <v>314</v>
       </c>
       <c r="C147" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D147" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E147" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4435,13 +4471,13 @@
         <v>315</v>
       </c>
       <c r="C148" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D148" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E148" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4452,13 +4488,13 @@
         <v>317</v>
       </c>
       <c r="C149" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D149" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E149" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4469,13 +4505,13 @@
         <v>316</v>
       </c>
       <c r="C150" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D150" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E150" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4486,13 +4522,13 @@
         <v>318</v>
       </c>
       <c r="C151" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D151" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E151" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4503,13 +4539,13 @@
         <v>313</v>
       </c>
       <c r="C152" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D152" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E152" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4520,13 +4556,13 @@
         <v>319</v>
       </c>
       <c r="C153" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D153" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E153" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4537,13 +4573,13 @@
         <v>320</v>
       </c>
       <c r="C154" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D154" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E154" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4554,13 +4590,13 @@
         <v>321</v>
       </c>
       <c r="C155" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D155" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E155" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4571,13 +4607,13 @@
         <v>322</v>
       </c>
       <c r="C156" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D156" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E156" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4588,55 +4624,55 @@
         <v>323</v>
       </c>
       <c r="C157" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D157" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E157" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C158" t="s">
-        <v>331</v>
-      </c>
-      <c r="D158" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="C158" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C159" t="s">
-        <v>331</v>
-      </c>
-      <c r="D159" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="C159" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C160" t="s">
-        <v>331</v>
-      </c>
-      <c r="D160" t="s">
-        <v>335</v>
+      <c r="C160" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4647,13 +4683,13 @@
         <v>324</v>
       </c>
       <c r="C161" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D161" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E161" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4664,13 +4700,13 @@
         <v>325</v>
       </c>
       <c r="C162" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D162" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E162" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4681,13 +4717,13 @@
         <v>326</v>
       </c>
       <c r="C163" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D163" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E163" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4698,13 +4734,13 @@
         <v>312</v>
       </c>
       <c r="C164" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D164" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E164" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4715,55 +4751,55 @@
         <v>312</v>
       </c>
       <c r="C165" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D165" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E165" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C166" t="s">
-        <v>331</v>
-      </c>
-      <c r="D166" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="C166" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C167" t="s">
-        <v>331</v>
-      </c>
-      <c r="D167" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="C167" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C168" t="s">
-        <v>331</v>
-      </c>
-      <c r="D168" t="s">
-        <v>335</v>
+      <c r="C168" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4771,16 +4807,16 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C169" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D169" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E169" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4788,16 +4824,16 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C170" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D170" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E170" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4805,16 +4841,16 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C171" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D171" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E171" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4822,16 +4858,16 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C172" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D172" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E172" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4839,16 +4875,16 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C173" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D173" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E173" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4856,16 +4892,16 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C174" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D174" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E174" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4873,16 +4909,16 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C175" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D175" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E175" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4890,16 +4926,16 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C176" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D176" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E176" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4907,16 +4943,16 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C177" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D177" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E177" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4924,16 +4960,16 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C178" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D178" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E178" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4941,16 +4977,16 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C179" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D179" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E179" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -4958,16 +4994,16 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C180" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D180" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E180" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -4978,90 +5014,90 @@
         <v>248</v>
       </c>
       <c r="C181" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D181" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E181" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B182" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C182" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="C182" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C183" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="C183" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C184" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="C184" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C185" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="C185" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C186" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="C186" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C187" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="C187" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B188" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C188" t="s">
-        <v>331</v>
+      <c r="C188" s="4" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5072,13 +5108,13 @@
         <v>249</v>
       </c>
       <c r="C189" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D189" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E189" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5089,27 +5125,27 @@
         <v>250</v>
       </c>
       <c r="C190" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D190" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E190" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C191" t="s">
-        <v>331</v>
-      </c>
-      <c r="D191" t="s">
-        <v>335</v>
+      <c r="C191" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5120,83 +5156,83 @@
         <v>251</v>
       </c>
       <c r="C192" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D192" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E192" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C193" t="s">
-        <v>331</v>
-      </c>
-      <c r="D193" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="C193" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C194" t="s">
-        <v>331</v>
-      </c>
-      <c r="D194" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="C194" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C195" t="s">
-        <v>331</v>
-      </c>
-      <c r="D195" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="C195" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C196" t="s">
-        <v>331</v>
-      </c>
-      <c r="D196" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="C196" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C197" t="s">
-        <v>331</v>
-      </c>
-      <c r="D197" t="s">
-        <v>335</v>
+      <c r="C197" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5207,69 +5243,69 @@
         <v>327</v>
       </c>
       <c r="C198" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D198" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E198" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C199" t="s">
-        <v>331</v>
-      </c>
-      <c r="D199" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+      <c r="C199" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C200" t="s">
-        <v>331</v>
-      </c>
-      <c r="D200" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+      <c r="C200" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B201" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C201" t="s">
-        <v>331</v>
-      </c>
-      <c r="D201" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+      <c r="C201" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C202" t="s">
-        <v>331</v>
-      </c>
-      <c r="D202" t="s">
-        <v>335</v>
+      <c r="C202" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5280,57 +5316,81 @@
         <v>252</v>
       </c>
       <c r="C203" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D203" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E203" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C204" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+      <c r="C204" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E204" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B205" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C205" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+      <c r="C205" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E205" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C206" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+      <c r="C206" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E206" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B207" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C207" t="s">
-        <v>331</v>
+      <c r="C207" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E207" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5341,21 +5401,21 @@
         <v>246</v>
       </c>
       <c r="C208" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E208" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+    <row r="209" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B209" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C209" t="s">
-        <v>331</v>
+      <c r="C209" s="4" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -5366,7 +5426,7 @@
         <v>328</v>
       </c>
       <c r="C210" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -5377,7 +5437,7 @@
         <v>328</v>
       </c>
       <c r="C211" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploy Platform on Azure article updated
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C5C2B4-B813-413E-AD06-29E405C58298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F52AF71-A539-462E-B8B2-2980C4FB940A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1057,9 +1057,6 @@
     <t>Create a new artilce /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module</t>
   </si>
   <si>
-    <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson3</t>
-  </si>
-  <si>
     <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson4</t>
   </si>
   <si>
@@ -1190,6 +1187,9 @@
   </si>
   <si>
     <t>platform/user-guide/elastic-app-search/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/Tutorials/creating-custom-module/</t>
   </si>
 </sst>
 </file>
@@ -1688,13 +1688,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2053,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A209" sqref="A209"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,10 +2186,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D13" t="s">
         <v>334</v>
@@ -2202,10 +2203,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D14" t="s">
         <v>334</v>
@@ -2219,10 +2220,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D15" t="s">
         <v>334</v>
@@ -2236,10 +2237,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D16" t="s">
         <v>334</v>
@@ -2253,10 +2254,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D17" t="s">
         <v>334</v>
@@ -2270,10 +2271,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D18" t="s">
         <v>334</v>
@@ -2287,10 +2288,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D19" t="s">
         <v>334</v>
@@ -2406,10 +2407,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D26" t="s">
         <v>334</v>
@@ -2423,10 +2424,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D27" t="s">
         <v>334</v>
@@ -2559,10 +2560,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C35" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D35" t="s">
         <v>334</v>
@@ -2987,7 +2988,7 @@
         <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D60" t="s">
         <v>334</v>
@@ -3001,10 +3002,10 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C61" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D61" t="s">
         <v>334</v>
@@ -3013,20 +3014,20 @@
         <v>342</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E62" s="4" t="s">
+      <c r="B62" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>342</v>
       </c>
     </row>
@@ -3035,7 +3036,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>330</v>
@@ -3052,10 +3053,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C64" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D64" t="s">
         <v>334</v>
@@ -3072,7 +3073,7 @@
         <v>250</v>
       </c>
       <c r="C65" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D65" t="s">
         <v>334</v>
@@ -3086,10 +3087,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C66" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D66" t="s">
         <v>334</v>
@@ -3103,7 +3104,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C67" t="s">
         <v>330</v>
@@ -3375,10 +3376,10 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C83" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D83" t="s">
         <v>334</v>
@@ -3392,10 +3393,10 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C84" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D84" t="s">
         <v>334</v>
@@ -3494,10 +3495,10 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C90" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D90" t="s">
         <v>334</v>
@@ -3528,10 +3529,10 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C92" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D92" t="s">
         <v>334</v>
@@ -3630,10 +3631,10 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C98" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D98" t="s">
         <v>334</v>
@@ -3647,10 +3648,10 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C99" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D99" t="s">
         <v>334</v>
@@ -3664,10 +3665,10 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C100" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D100" t="s">
         <v>334</v>
@@ -3681,10 +3682,10 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C101" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D101" t="s">
         <v>334</v>
@@ -3698,10 +3699,10 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C102" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D102" t="s">
         <v>334</v>
@@ -3715,10 +3716,10 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C103" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D103" t="s">
         <v>334</v>
@@ -3732,10 +3733,10 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C104" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D104" t="s">
         <v>334</v>
@@ -3749,10 +3750,10 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C105" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D105" t="s">
         <v>334</v>
@@ -3794,7 +3795,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C108" t="s">
         <v>330</v>
@@ -3961,10 +3962,10 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C118" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D118" t="s">
         <v>334</v>
@@ -4230,10 +4231,10 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C134" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D134" t="s">
         <v>334</v>
@@ -4417,10 +4418,10 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C145" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D145" t="s">
         <v>334</v>
@@ -4807,10 +4808,10 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C169" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D169" t="s">
         <v>334</v>
@@ -4824,10 +4825,10 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C170" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D170" t="s">
         <v>334</v>
@@ -4841,10 +4842,10 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C171" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D171" t="s">
         <v>334</v>
@@ -4858,10 +4859,10 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C172" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D172" t="s">
         <v>334</v>
@@ -4875,10 +4876,10 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C173" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D173" t="s">
         <v>334</v>
@@ -4892,10 +4893,10 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C174" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D174" t="s">
         <v>334</v>
@@ -4909,10 +4910,10 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C175" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D175" t="s">
         <v>334</v>
@@ -4926,10 +4927,10 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C176" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D176" t="s">
         <v>334</v>
@@ -4943,10 +4944,10 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C177" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D177" t="s">
         <v>334</v>
@@ -4960,10 +4961,10 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C178" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D178" t="s">
         <v>334</v>
@@ -4977,10 +4978,10 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C179" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D179" t="s">
         <v>334</v>
@@ -4994,10 +4995,10 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C180" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D180" t="s">
         <v>334</v>
@@ -5014,7 +5015,7 @@
         <v>248</v>
       </c>
       <c r="C181" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D181" t="s">
         <v>334</v>
@@ -5108,7 +5109,7 @@
         <v>249</v>
       </c>
       <c r="C189" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D189" t="s">
         <v>334</v>
@@ -5125,7 +5126,7 @@
         <v>250</v>
       </c>
       <c r="C190" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D190" t="s">
         <v>334</v>
@@ -5156,7 +5157,7 @@
         <v>251</v>
       </c>
       <c r="C192" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D192" t="s">
         <v>334</v>
@@ -5243,7 +5244,7 @@
         <v>327</v>
       </c>
       <c r="C198" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D198" t="s">
         <v>334</v>
@@ -5316,7 +5317,7 @@
         <v>252</v>
       </c>
       <c r="C203" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D203" t="s">
         <v>334</v>
@@ -5333,7 +5334,7 @@
         <v>253</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D204" s="4" t="s">
         <v>334</v>
@@ -5350,7 +5351,7 @@
         <v>254</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D205" s="4" t="s">
         <v>334</v>
@@ -5367,7 +5368,7 @@
         <v>255</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D206" s="4" t="s">
         <v>334</v>
@@ -5384,7 +5385,7 @@
         <v>256</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D207" s="4" t="s">
         <v>334</v>

</xml_diff>

<commit_message>
Return, Shipping, Shipstation modules descriptions added
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F52AF71-A539-462E-B8B2-2980C4FB940A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B79A96-97A2-440A-9F95-E8EAB61CD893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="393">
   <si>
     <t>Original Url</t>
   </si>
@@ -1190,6 +1190,15 @@
   </si>
   <si>
     <t>platform/developer-guide/Tutorials-and-How-tos/Tutorials/creating-custom-module/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/shipstation/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/shipping/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/return/overview/</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1697,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1696,6 +1705,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2054,8 +2064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3762,15 +3772,18 @@
         <v>342</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="C106" t="s">
-        <v>330</v>
+      <c r="C106" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4634,46 +4647,55 @@
         <v>336</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
+    <row r="158" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B158" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C158" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D158" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="4" t="s">
+      <c r="B158" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C158" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B159" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D159" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="4" t="s">
+      <c r="B159" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C159" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D159" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E159" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B160" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D160" s="4" t="s">
-        <v>334</v>
+      <c r="B160" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="D160" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4774,6 +4796,9 @@
       <c r="D166" s="4" t="s">
         <v>334</v>
       </c>
+      <c r="E166" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
@@ -4788,6 +4813,9 @@
       <c r="D167" s="4" t="s">
         <v>334</v>
       </c>
+      <c r="E167" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
@@ -4802,6 +4830,9 @@
       <c r="D168" s="4" t="s">
         <v>334</v>
       </c>
+      <c r="E168" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
@@ -4974,7 +5005,7 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+      <c r="A179" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B179" t="s">
@@ -5034,6 +5065,12 @@
       <c r="C182" s="4" t="s">
         <v>330</v>
       </c>
+      <c r="D182" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E182" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="183" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
@@ -5045,6 +5082,12 @@
       <c r="C183" s="4" t="s">
         <v>330</v>
       </c>
+      <c r="D183" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E183" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="184" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
@@ -5056,6 +5099,12 @@
       <c r="C184" s="4" t="s">
         <v>330</v>
       </c>
+      <c r="D184" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E184" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="185" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
@@ -5067,6 +5116,12 @@
       <c r="C185" s="4" t="s">
         <v>330</v>
       </c>
+      <c r="D185" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E185" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="186" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
@@ -5078,6 +5133,12 @@
       <c r="C186" s="4" t="s">
         <v>330</v>
       </c>
+      <c r="D186" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E186" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="187" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
@@ -5089,6 +5150,12 @@
       <c r="C187" s="4" t="s">
         <v>330</v>
       </c>
+      <c r="D187" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E187" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="188" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
@@ -5100,6 +5167,12 @@
       <c r="C188" s="4" t="s">
         <v>330</v>
       </c>
+      <c r="D188" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E188" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
@@ -5326,71 +5399,71 @@
         <v>342</v>
       </c>
     </row>
-    <row r="204" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="4" t="s">
+    <row r="204" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B204" s="4" t="s">
+      <c r="B204" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C204" s="4" t="s">
+      <c r="C204" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="D204" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E204" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="4" t="s">
+      <c r="D204" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E204" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="B205" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="C205" s="4" t="s">
+      <c r="C205" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="D205" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E205" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="4" t="s">
+      <c r="D205" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E205" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B206" s="4" t="s">
+      <c r="B206" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="C206" s="4" t="s">
+      <c r="C206" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="D206" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E206" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="4" t="s">
+      <c r="D206" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E206" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B207" s="4" t="s">
+      <c r="B207" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C207" s="4" t="s">
+      <c r="C207" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="D207" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E207" s="4" t="s">
+      <c r="D207" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E207" s="6" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5408,7 +5481,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>209</v>
       </c>
@@ -5418,8 +5491,11 @@
       <c r="C209" s="4" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D209" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>210</v>
       </c>
@@ -5430,7 +5506,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>211</v>
       </c>
@@ -5483,6 +5559,7 @@
     <hyperlink ref="A134" r:id="rId30" xr:uid="{16F8ED4E-A2AF-433A-BC67-2DB462120B1B}"/>
     <hyperlink ref="A158" r:id="rId31" xr:uid="{27210CD7-8CAB-47C6-B488-A8E7B95F5B2C}"/>
     <hyperlink ref="A103" r:id="rId32" xr:uid="{9B568E95-26EE-4D47-B494-E1484996E56D}"/>
+    <hyperlink ref="A179" r:id="rId33" xr:uid="{BF55F26A-1F68-4921-BAE8-061100358C7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added and updated Scalability, Tutorials and How-tos, Platform Manager, Elastic Search 8, Event bus and other segments
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B79A96-97A2-440A-9F95-E8EAB61CD893}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F852F1CE-DD72-4804-A600-D3228D0A3E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="400">
   <si>
     <t>Original Url</t>
   </si>
@@ -1054,12 +1054,6 @@
     <t>platform/developer-guide/Fundamentals/Dynamic-Properties/overview</t>
   </si>
   <si>
-    <t>Create a new artilce /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module</t>
-  </si>
-  <si>
-    <t>Verify and copy content  to /platform/developer-guide/Tutorials-and-How-tos/Lessons/Create-Customer-Review-module/lesson4</t>
-  </si>
-  <si>
     <t>OnReview</t>
   </si>
   <si>
@@ -1199,6 +1193,33 @@
   </si>
   <si>
     <t>platform/user-guide/return/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/tax/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/webhooks/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/assets/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/health-checks/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/user-profile/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/event-bus/overview/</t>
+  </si>
+  <si>
+    <t>platform/user-guide/subscriptions/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/overview/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/Tutorials/build-platform-manager-ui/</t>
   </si>
 </sst>
 </file>
@@ -1697,11 +1718,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2064,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A187" sqref="A187"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,10 +2216,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C13" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D13" t="s">
         <v>334</v>
@@ -2213,10 +2233,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D14" t="s">
         <v>334</v>
@@ -2230,10 +2250,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D15" t="s">
         <v>334</v>
@@ -2247,10 +2267,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C16" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D16" t="s">
         <v>334</v>
@@ -2264,10 +2284,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D17" t="s">
         <v>334</v>
@@ -2281,10 +2301,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C18" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D18" t="s">
         <v>334</v>
@@ -2298,10 +2318,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C19" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D19" t="s">
         <v>334</v>
@@ -2417,10 +2437,10 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C26" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D26" t="s">
         <v>334</v>
@@ -2434,10 +2454,10 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C27" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D27" t="s">
         <v>334</v>
@@ -2570,10 +2590,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C35" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D35" t="s">
         <v>334</v>
@@ -2973,20 +2993,20 @@
         <v>336</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E59" s="4" t="s">
+      <c r="B59" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>342</v>
       </c>
     </row>
@@ -2998,7 +3018,7 @@
         <v>219</v>
       </c>
       <c r="C60" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D60" t="s">
         <v>334</v>
@@ -3012,10 +3032,10 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C61" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D61" t="s">
         <v>334</v>
@@ -3024,37 +3044,37 @@
         <v>342</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+    <row r="62" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="B62" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E63" s="4" t="s">
+      <c r="B63" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>342</v>
       </c>
     </row>
@@ -3063,10 +3083,10 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C64" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D64" t="s">
         <v>334</v>
@@ -3083,7 +3103,7 @@
         <v>250</v>
       </c>
       <c r="C65" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D65" t="s">
         <v>334</v>
@@ -3097,10 +3117,10 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C66" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D66" t="s">
         <v>334</v>
@@ -3114,7 +3134,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C67" t="s">
         <v>330</v>
@@ -3386,10 +3406,10 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C83" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D83" t="s">
         <v>334</v>
@@ -3403,10 +3423,10 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C84" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D84" t="s">
         <v>334</v>
@@ -3505,10 +3525,10 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C90" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D90" t="s">
         <v>334</v>
@@ -3539,10 +3559,10 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C92" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D92" t="s">
         <v>334</v>
@@ -3641,10 +3661,10 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C98" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D98" t="s">
         <v>334</v>
@@ -3658,10 +3678,10 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C99" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D99" t="s">
         <v>334</v>
@@ -3675,10 +3695,10 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C100" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D100" t="s">
         <v>334</v>
@@ -3692,10 +3712,10 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C101" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D101" t="s">
         <v>334</v>
@@ -3709,10 +3729,10 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C102" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D102" t="s">
         <v>334</v>
@@ -3726,10 +3746,10 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C103" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D103" t="s">
         <v>334</v>
@@ -3743,10 +3763,10 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C104" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D104" t="s">
         <v>334</v>
@@ -3760,10 +3780,10 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C105" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D105" t="s">
         <v>334</v>
@@ -3772,18 +3792,21 @@
         <v>342</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+    <row r="106" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>334</v>
+      <c r="B106" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3808,7 +3831,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C108" t="s">
         <v>330</v>
@@ -3975,10 +3998,10 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C118" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D118" t="s">
         <v>334</v>
@@ -4244,10 +4267,10 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C134" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D134" t="s">
         <v>334</v>
@@ -4431,10 +4454,10 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C145" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D145" t="s">
         <v>334</v>
@@ -4647,54 +4670,54 @@
         <v>336</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="7" t="s">
+    <row r="158" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B158" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E158" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="6" t="s">
+      <c r="B158" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E158" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B159" s="6" t="s">
-        <v>391</v>
-      </c>
-      <c r="C159" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D159" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E159" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="6" t="s">
+      <c r="B159" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D159" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E159" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B160" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="C160" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D160" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="E160" s="6" t="s">
+      <c r="B160" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D160" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E160" s="5" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4783,54 +4806,54 @@
         <v>336</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="4" t="s">
+    <row r="166" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B166" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C166" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D166" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E166" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="4" t="s">
+      <c r="B166" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B167" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C167" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E167" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
+      <c r="B167" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D167" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E167" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B168" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D168" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E168" t="s">
+      <c r="B168" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E168" s="5" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4839,10 +4862,10 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C169" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D169" t="s">
         <v>334</v>
@@ -4856,10 +4879,10 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C170" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D170" t="s">
         <v>334</v>
@@ -4873,10 +4896,10 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C171" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D171" t="s">
         <v>334</v>
@@ -4890,10 +4913,10 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C172" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D172" t="s">
         <v>334</v>
@@ -4907,10 +4930,10 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C173" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D173" t="s">
         <v>334</v>
@@ -4924,10 +4947,10 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C174" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D174" t="s">
         <v>334</v>
@@ -4941,10 +4964,10 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C175" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D175" t="s">
         <v>334</v>
@@ -4958,10 +4981,10 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C176" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D176" t="s">
         <v>334</v>
@@ -4975,10 +4998,10 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C177" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D177" t="s">
         <v>334</v>
@@ -4992,10 +5015,10 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C178" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D178" t="s">
         <v>334</v>
@@ -5009,10 +5032,10 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C179" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D179" t="s">
         <v>334</v>
@@ -5026,10 +5049,10 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C180" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D180" t="s">
         <v>334</v>
@@ -5046,7 +5069,7 @@
         <v>248</v>
       </c>
       <c r="C181" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D181" t="s">
         <v>334</v>
@@ -5055,119 +5078,119 @@
         <v>342</v>
       </c>
     </row>
-    <row r="182" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="4" t="s">
+    <row r="182" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B182" s="5" t="s">
+      <c r="B182" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C182" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D182" s="4" t="s">
+      <c r="C182" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D182" s="3" t="s">
         <v>334</v>
       </c>
       <c r="E182" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="183" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="4" t="s">
+    <row r="183" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B183" s="5" t="s">
+      <c r="B183" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C183" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D183" s="4" t="s">
+      <c r="C183" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D183" s="3" t="s">
         <v>334</v>
       </c>
       <c r="E183" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="184" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="4" t="s">
+    <row r="184" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B184" s="5" t="s">
+      <c r="B184" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C184" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D184" s="4" t="s">
+      <c r="C184" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D184" s="3" t="s">
         <v>334</v>
       </c>
       <c r="E184" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="185" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="4" t="s">
+    <row r="185" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B185" s="5" t="s">
+      <c r="B185" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C185" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D185" s="4" t="s">
+      <c r="C185" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D185" s="3" t="s">
         <v>334</v>
       </c>
       <c r="E185" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="186" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="4" t="s">
+    <row r="186" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B186" s="5" t="s">
+      <c r="B186" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C186" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D186" s="4" t="s">
+      <c r="C186" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D186" s="3" t="s">
         <v>334</v>
       </c>
       <c r="E186" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="187" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="4" t="s">
+    <row r="187" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B187" s="5" t="s">
+      <c r="B187" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C187" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D187" s="4" t="s">
+      <c r="C187" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D187" s="3" t="s">
         <v>334</v>
       </c>
       <c r="E187" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="188" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="4" t="s">
+    <row r="188" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B188" s="5" t="s">
+      <c r="B188" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C188" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D188" s="4" t="s">
+      <c r="C188" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D188" s="3" t="s">
         <v>334</v>
       </c>
       <c r="E188" t="s">
@@ -5182,7 +5205,7 @@
         <v>249</v>
       </c>
       <c r="C189" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D189" t="s">
         <v>334</v>
@@ -5199,7 +5222,7 @@
         <v>250</v>
       </c>
       <c r="C190" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D190" t="s">
         <v>334</v>
@@ -5208,17 +5231,17 @@
         <v>342</v>
       </c>
     </row>
-    <row r="191" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="4" t="s">
+    <row r="191" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B191" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C191" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D191" s="4" t="s">
+      <c r="C191" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D191" s="3" t="s">
         <v>334</v>
       </c>
     </row>
@@ -5230,7 +5253,7 @@
         <v>251</v>
       </c>
       <c r="C192" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D192" t="s">
         <v>334</v>
@@ -5239,73 +5262,76 @@
         <v>342</v>
       </c>
     </row>
-    <row r="193" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="4" t="s">
+    <row r="193" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B193" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C193" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D193" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="4" t="s">
+      <c r="C193" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B194" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C194" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D194" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="4" t="s">
+      <c r="C194" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B195" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C195" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D195" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="4" t="s">
+      <c r="C195" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="B196" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="C196" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D196" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E196" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B197" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C196" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D196" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="B197" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C197" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D197" s="4" t="s">
+      <c r="C197" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D197" s="3" t="s">
         <v>334</v>
       </c>
     </row>
@@ -5317,7 +5343,7 @@
         <v>327</v>
       </c>
       <c r="C198" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D198" t="s">
         <v>334</v>
@@ -5326,60 +5352,63 @@
         <v>342</v>
       </c>
     </row>
-    <row r="199" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="4" t="s">
+    <row r="199" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B199" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C199" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D199" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="4" t="s">
+      <c r="C199" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B200" s="4" t="s">
+      <c r="B200" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C200" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D200" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="4" t="s">
+      <c r="C200" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="B201" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C201" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D201" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="4" t="s">
+      <c r="C201" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B202" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C202" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D202" s="4" t="s">
-        <v>334</v>
+      <c r="B202" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E202" s="5" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5390,7 +5419,7 @@
         <v>252</v>
       </c>
       <c r="C203" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D203" t="s">
         <v>334</v>
@@ -5399,71 +5428,71 @@
         <v>342</v>
       </c>
     </row>
-    <row r="204" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="6" t="s">
+    <row r="204" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B204" s="6" t="s">
+      <c r="B204" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="C204" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D204" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E204" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="6" t="s">
+      <c r="C204" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D204" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E204" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B205" s="6" t="s">
+      <c r="B205" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C205" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D205" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E205" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="6" t="s">
+      <c r="C205" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E205" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B206" s="6" t="s">
+      <c r="B206" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="C206" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D206" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E206" s="6" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="6" t="s">
+      <c r="C206" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D206" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E206" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B207" s="6" t="s">
+      <c r="B207" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C207" s="6" t="s">
-        <v>346</v>
-      </c>
-      <c r="D207" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="E207" s="6" t="s">
+      <c r="C207" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D207" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E207" s="5" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5481,21 +5510,24 @@
         <v>257</v>
       </c>
     </row>
-    <row r="209" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="4" t="s">
+    <row r="209" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B209" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C209" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D209" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B209" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C209" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E209" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>210</v>
       </c>
@@ -5506,7 +5538,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>211</v>
       </c>
@@ -5562,5 +5594,6 @@
     <hyperlink ref="A179" r:id="rId33" xr:uid="{BF55F26A-1F68-4921-BAE8-061100358C7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Extending database model , Generating pdfs, JWT authorization articles added
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F852F1CE-DD72-4804-A600-D3228D0A3E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EE6101-0F34-4EB1-8A1F-FCF1CD38889B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="408">
   <si>
     <t>Original Url</t>
   </si>
@@ -1220,6 +1220,30 @@
   </si>
   <si>
     <t>platform/developer-guide/Tutorials-and-How-tos/Tutorials/build-platform-manager-ui/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Platform-Manager/localization/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/upgrading-to-net8/</t>
+  </si>
+  <si>
+    <t>Oleg said these articles should be placed into some sort of archive.</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Fundamentals/Scalability/scalability-options/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/type-inheritance-support-in-swagger/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/Tutorials/extending-database-model/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/generating-pdfs/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/authorization-using-jwt/</t>
   </si>
 </sst>
 </file>
@@ -1723,9 +1747,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2084,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,7 +2146,13 @@
         <v>247</v>
       </c>
       <c r="C2" t="s">
-        <v>330</v>
+        <v>344</v>
+      </c>
+      <c r="D2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2133,7 +2163,13 @@
         <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>330</v>
+        <v>344</v>
+      </c>
+      <c r="D3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2144,7 +2180,13 @@
         <v>219</v>
       </c>
       <c r="C4" t="s">
-        <v>330</v>
+        <v>344</v>
+      </c>
+      <c r="D4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E4" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2993,20 +3035,20 @@
         <v>336</v>
       </c>
     </row>
-    <row r="59" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+    <row r="59" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E59" s="5" t="s">
+      <c r="C59" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -3044,37 +3086,37 @@
         <v>342</v>
       </c>
     </row>
-    <row r="62" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="62" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+      <c r="C62" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>330</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E63" s="5" t="s">
+      <c r="C63" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -3792,20 +3834,20 @@
         <v>342</v>
       </c>
     </row>
-    <row r="106" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="C106" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E106" s="5" t="s">
+      <c r="C106" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E106" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4670,54 +4712,54 @@
         <v>336</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="6" t="s">
+    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="B158" s="5" t="s">
+      <c r="B158" s="4" t="s">
         <v>390</v>
       </c>
-      <c r="C158" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D158" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E158" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
+      <c r="C158" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B159" s="5" t="s">
+      <c r="B159" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="C159" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D159" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E159" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
+      <c r="C159" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B160" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="C160" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D160" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="E160" s="5" t="s">
+      <c r="C160" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E160" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -4806,54 +4848,54 @@
         <v>336</v>
       </c>
     </row>
-    <row r="166" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
+    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="B166" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="C166" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D166" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E166" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
+      <c r="C166" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B167" s="5" t="s">
+      <c r="B167" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="C167" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D167" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E167" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="5" t="s">
+      <c r="C167" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E167" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B168" s="5" t="s">
+      <c r="B168" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="C168" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D168" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E168" s="5" t="s">
+      <c r="C168" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E168" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5078,122 +5120,89 @@
         <v>342</v>
       </c>
     </row>
-    <row r="182" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="3" t="s">
+    <row r="182" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B182" s="4" t="s">
+      <c r="B182" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C182" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D182" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E182" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
+      <c r="C182" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E182" s="4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B183" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C183" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E183" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="3" t="s">
+      <c r="C183" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B184" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C184" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D184" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E184" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="3" t="s">
+      <c r="C184" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B185" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C185" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D185" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E185" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="3" t="s">
+      <c r="C185" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B186" s="4" t="s">
+      <c r="B186" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C186" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E186" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="3" t="s">
+      <c r="C186" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="B187" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C187" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D187" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E187" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="3" t="s">
+      <c r="C187" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B188" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D188" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E188" t="s">
+      <c r="B188" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D188" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E188" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5231,18 +5240,21 @@
         <v>342</v>
       </c>
     </row>
-    <row r="191" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="3" t="s">
+    <row r="191" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B191" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D191" s="3" t="s">
-        <v>334</v>
+      <c r="B191" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E191" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5262,77 +5274,89 @@
         <v>342</v>
       </c>
     </row>
-    <row r="193" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="3" t="s">
+    <row r="193" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="B193" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D193" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="3" t="s">
+      <c r="B193" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E193" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B194" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D194" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="3" t="s">
+      <c r="B194" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E194" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B195" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D195" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="5" t="s">
+      <c r="B195" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E195" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B196" s="5" t="s">
+      <c r="B196" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C196" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D196" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E196" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="3" t="s">
+      <c r="C196" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B197" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D197" s="3" t="s">
-        <v>334</v>
+      <c r="B197" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E197" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5352,18 +5376,21 @@
         <v>342</v>
       </c>
     </row>
-    <row r="199" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="3" t="s">
+    <row r="199" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B199" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D199" s="3" t="s">
-        <v>334</v>
+      <c r="B199" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E199" s="4" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="200" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5394,20 +5421,20 @@
         <v>334</v>
       </c>
     </row>
-    <row r="202" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="5" t="s">
+    <row r="202" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="B202" s="5" t="s">
+      <c r="B202" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="C202" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D202" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E202" s="5" t="s">
+      <c r="C202" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E202" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5428,71 +5455,71 @@
         <v>342</v>
       </c>
     </row>
-    <row r="204" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="5" t="s">
+    <row r="204" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B204" s="5" t="s">
+      <c r="B204" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="C204" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D204" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E204" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="5" t="s">
+      <c r="C204" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E204" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B205" s="5" t="s">
+      <c r="B205" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C205" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D205" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E205" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="5" t="s">
+      <c r="C205" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E205" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B206" s="5" t="s">
+      <c r="B206" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C206" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D206" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E206" s="5" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="5" t="s">
+      <c r="C206" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E206" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B207" s="5" t="s">
+      <c r="B207" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C207" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D207" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E207" s="5" t="s">
+      <c r="C207" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E207" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5510,20 +5537,20 @@
         <v>257</v>
       </c>
     </row>
-    <row r="209" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="5" t="s">
+    <row r="209" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B209" s="5" t="s">
+      <c r="B209" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="C209" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="D209" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="E209" s="5" t="s">
+      <c r="C209" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E209" s="4" t="s">
         <v>342</v>
       </c>
     </row>
@@ -5531,22 +5558,28 @@
       <c r="A210" t="s">
         <v>210</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C210" t="s">
+        <v>330</v>
+      </c>
+      <c r="E210" t="s">
         <v>328</v>
-      </c>
-      <c r="C210" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>211</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C211" t="s">
+        <v>330</v>
+      </c>
+      <c r="E211" t="s">
         <v>328</v>
-      </c>
-      <c r="C211" t="s">
-        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tutorials and How-tos extended with new articles
</commit_message>
<xml_diff>
--- a/sitemap/docs_virtocommerce_org-sitemap.xlsx
+++ b/sitemap/docs_virtocommerce_org-sitemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Virto\vc-docs\sitemap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EE6101-0F34-4EB1-8A1F-FCF1CD38889B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84392553-2DEC-4C26-A6C2-1DCD703E4B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="409">
   <si>
     <t>Original Url</t>
   </si>
@@ -658,9 +658,6 @@
     <t>https://docs.virtocommerce.org/versions/3.0/</t>
   </si>
   <si>
-    <t>Need to add a new article from previous docs</t>
-  </si>
-  <si>
     <t>https://help.virtocommerce.com/support/home</t>
   </si>
   <si>
@@ -1244,6 +1241,12 @@
   </si>
   <si>
     <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/authorization-using-jwt/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/user-email-verification/</t>
+  </si>
+  <si>
+    <t>platform/developer-guide/Tutorials-and-How-tos/How-tos/sharing-bearer-tokens/</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1397,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1574,12 +1577,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1742,11 +1739,10 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
@@ -2108,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200:XFD200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,13 +2125,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2143,16 +2139,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2160,16 +2156,16 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2177,16 +2173,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2194,7 +2190,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2202,7 +2198,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2210,7 +2206,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2218,7 +2214,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2226,7 +2222,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2234,7 +2230,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2242,7 +2238,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2250,7 +2246,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2258,16 +2254,16 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E13" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2275,16 +2271,16 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2292,16 +2288,16 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2309,16 +2305,16 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2326,16 +2322,16 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2343,16 +2339,16 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2360,16 +2356,16 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2377,16 +2373,16 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,16 +2390,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D21" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2411,16 +2407,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2428,16 +2424,16 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2445,16 +2441,16 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D24" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2462,16 +2458,16 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2479,16 +2475,16 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C26" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2496,16 +2492,16 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2513,16 +2509,16 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2530,16 +2526,16 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2547,16 +2543,16 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2564,16 +2560,16 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E31" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2581,16 +2577,16 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D32" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2598,16 +2594,16 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C33" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2615,16 +2611,16 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C34" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2632,16 +2628,16 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C35" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E35" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2649,16 +2645,16 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,16 +2662,16 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C37" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D37" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2683,16 +2679,16 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C38" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D38" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E38" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2700,16 +2696,16 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C39" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D39" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2717,16 +2713,16 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C40" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D40" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2734,16 +2730,16 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2751,16 +2747,16 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C42" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D42" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E42" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2768,16 +2764,16 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C43" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D43" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E43" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2785,16 +2781,16 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C44" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2802,16 +2798,16 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C45" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D45" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2819,16 +2815,16 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C46" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D46" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2836,16 +2832,16 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C47" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D47" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,16 +2849,16 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C48" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D48" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2870,16 +2866,16 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C49" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D49" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E49" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2887,16 +2883,16 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C50" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E50" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2904,16 +2900,16 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C51" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D51" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E51" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2921,16 +2917,16 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C52" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E52" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2938,16 +2934,16 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C53" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E53" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2955,16 +2951,16 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C54" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D54" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E54" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2972,16 +2968,16 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C55" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D55" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E55" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2989,16 +2985,16 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C56" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D56" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E56" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3006,16 +3002,16 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C57" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E57" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3023,33 +3019,33 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C58" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D58" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E58" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>398</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>342</v>
+      <c r="B59" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3057,16 +3053,16 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C60" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D60" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E60" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3074,50 +3070,50 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C61" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D61" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E61" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="B62" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B63" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>342</v>
+      <c r="B63" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3125,16 +3121,16 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D64" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E64" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3142,16 +3138,16 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C65" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D65" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E65" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3159,16 +3155,16 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C66" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D66" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E66" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3176,16 +3172,16 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C67" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D67" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E67" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3193,16 +3189,16 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C68" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D68" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E68" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3210,16 +3206,16 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C69" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D69" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E69" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3227,16 +3223,16 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C70" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D70" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E70" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3244,16 +3240,16 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C71" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E71" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3261,16 +3257,16 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C72" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D72" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3278,16 +3274,16 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C73" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D73" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E73" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3295,16 +3291,16 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C74" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D74" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E74" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3312,16 +3308,16 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C75" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3329,16 +3325,16 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C76" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D76" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E76" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3346,16 +3342,16 @@
         <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C77" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E77" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3363,16 +3359,16 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C78" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D78" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E78" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3380,16 +3376,16 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C79" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D79" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E79" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3397,16 +3393,16 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C80" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D80" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E80" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3414,16 +3410,16 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C81" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D81" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E81" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3431,16 +3427,16 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C82" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D82" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E82" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3448,16 +3444,16 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C83" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D83" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E83" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3465,16 +3461,16 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C84" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D84" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E84" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3482,16 +3478,16 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C85" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D85" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E85" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3499,16 +3495,16 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C86" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D86" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E86" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3516,16 +3512,16 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C87" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D87" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E87" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3533,16 +3529,16 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C88" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D88" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E88" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3550,16 +3546,16 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C89" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D89" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E89" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3567,16 +3563,16 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C90" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D90" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E90" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3584,16 +3580,16 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C91" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D91" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E91" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3601,16 +3597,16 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C92" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D92" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E92" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3618,16 +3614,16 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C93" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D93" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E93" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3635,16 +3631,16 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C94" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D94" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E94" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3652,16 +3648,16 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C95" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D95" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E95" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3669,16 +3665,16 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C96" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D96" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E96" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3686,16 +3682,16 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C97" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D97" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E97" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3703,16 +3699,16 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C98" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D98" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E98" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3720,16 +3716,16 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C99" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D99" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3737,16 +3733,16 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C100" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D100" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E100" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3754,16 +3750,16 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C101" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D101" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3771,16 +3767,16 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C102" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D102" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E102" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3788,16 +3784,16 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C103" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D103" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E103" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3805,16 +3801,16 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C104" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D104" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E104" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3822,33 +3818,33 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C105" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D105" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E105" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E106" s="4" t="s">
-        <v>342</v>
+      <c r="B106" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3856,16 +3852,16 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C107" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D107" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E107" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3873,16 +3869,16 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C108" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D108" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E108" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3890,16 +3886,16 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C109" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D109" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E109" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3907,13 +3903,13 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C110" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D110" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3921,16 +3917,16 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C111" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D111" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E111" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3938,16 +3934,16 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C112" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D112" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E112" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3955,16 +3951,16 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C113" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D113" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E113" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3972,16 +3968,16 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C114" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D114" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E114" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3989,16 +3985,16 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C115" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D115" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E115" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4006,16 +4002,16 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C116" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D116" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E116" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4023,16 +4019,16 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C117" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D117" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E117" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4040,16 +4036,16 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C118" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D118" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E118" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4057,16 +4053,16 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C119" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D119" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E119" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4074,16 +4070,16 @@
         <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C120" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D120" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E120" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4091,16 +4087,16 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C121" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D121" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E121" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4108,16 +4104,16 @@
         <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C122" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D122" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E122" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4125,16 +4121,16 @@
         <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C123" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D123" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E123" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4142,16 +4138,16 @@
         <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C124" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D124" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E124" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4159,16 +4155,16 @@
         <v>125</v>
       </c>
       <c r="B125" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C125" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D125" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E125" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4176,16 +4172,16 @@
         <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C126" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D126" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E126" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4193,16 +4189,16 @@
         <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C127" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D127" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E127" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4210,16 +4206,16 @@
         <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C128" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D128" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E128" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4227,16 +4223,16 @@
         <v>129</v>
       </c>
       <c r="B129" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C129" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D129" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E129" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4244,16 +4240,16 @@
         <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C130" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D130" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E130" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4261,16 +4257,16 @@
         <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C131" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D131" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E131" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4278,13 +4274,13 @@
         <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C132" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D132" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4292,16 +4288,16 @@
         <v>133</v>
       </c>
       <c r="B133" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C133" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D133" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E133" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4309,16 +4305,16 @@
         <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C134" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D134" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E134" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4326,16 +4322,16 @@
         <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C135" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D135" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E135" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4343,16 +4339,16 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C136" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D136" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E136" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4360,16 +4356,16 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C137" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D137" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E137" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4377,16 +4373,16 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C138" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D138" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E138" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4394,16 +4390,16 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C139" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D139" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E139" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4411,16 +4407,16 @@
         <v>140</v>
       </c>
       <c r="B140" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C140" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D140" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E140" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4428,16 +4424,16 @@
         <v>141</v>
       </c>
       <c r="B141" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C141" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D141" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E141" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4445,16 +4441,16 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C142" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D142" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E142" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4462,16 +4458,16 @@
         <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C143" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D143" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E143" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4479,16 +4475,16 @@
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C144" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D144" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E144" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4496,16 +4492,16 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C145" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D145" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E145" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4513,16 +4509,16 @@
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C146" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D146" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E146" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4530,16 +4526,16 @@
         <v>147</v>
       </c>
       <c r="B147" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C147" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D147" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E147" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4547,16 +4543,16 @@
         <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C148" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D148" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E148" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4564,16 +4560,16 @@
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C149" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D149" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E149" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4581,16 +4577,16 @@
         <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C150" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D150" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E150" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4598,16 +4594,16 @@
         <v>151</v>
       </c>
       <c r="B151" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C151" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D151" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E151" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4615,16 +4611,16 @@
         <v>152</v>
       </c>
       <c r="B152" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C152" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D152" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E152" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4632,16 +4628,16 @@
         <v>153</v>
       </c>
       <c r="B153" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C153" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D153" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E153" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4649,16 +4645,16 @@
         <v>154</v>
       </c>
       <c r="B154" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C154" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D154" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E154" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4666,16 +4662,16 @@
         <v>155</v>
       </c>
       <c r="B155" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C155" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D155" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E155" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4683,16 +4679,16 @@
         <v>156</v>
       </c>
       <c r="B156" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C156" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D156" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E156" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4700,67 +4696,67 @@
         <v>157</v>
       </c>
       <c r="B157" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C157" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D157" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E157" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B158" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="C158" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D158" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E158" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="4" t="s">
+      <c r="B158" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B159" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D159" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="4" t="s">
+      <c r="B159" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B160" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D160" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="E160" s="4" t="s">
-        <v>342</v>
+      <c r="B160" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4768,16 +4764,16 @@
         <v>161</v>
       </c>
       <c r="B161" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C161" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D161" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E161" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4785,16 +4781,16 @@
         <v>162</v>
       </c>
       <c r="B162" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C162" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D162" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E162" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4802,16 +4798,16 @@
         <v>163</v>
       </c>
       <c r="B163" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C163" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D163" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E163" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -4819,16 +4815,16 @@
         <v>164</v>
       </c>
       <c r="B164" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C164" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D164" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E164" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -4836,67 +4832,67 @@
         <v>165</v>
       </c>
       <c r="B165" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C165" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D165" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E165" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B166" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="C166" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D166" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E166" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="4" t="s">
+      <c r="B166" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B167" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B168" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="C167" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E167" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D168" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E168" s="4" t="s">
-        <v>342</v>
+      <c r="C168" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -4904,16 +4900,16 @@
         <v>169</v>
       </c>
       <c r="B169" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C169" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D169" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E169" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4921,16 +4917,16 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C170" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D170" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E170" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4938,16 +4934,16 @@
         <v>171</v>
       </c>
       <c r="B171" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C171" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D171" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E171" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4955,16 +4951,16 @@
         <v>172</v>
       </c>
       <c r="B172" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C172" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D172" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E172" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4972,16 +4968,16 @@
         <v>173</v>
       </c>
       <c r="B173" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C173" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D173" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E173" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4989,16 +4985,16 @@
         <v>174</v>
       </c>
       <c r="B174" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C174" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D174" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E174" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -5006,16 +5002,16 @@
         <v>175</v>
       </c>
       <c r="B175" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C175" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D175" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E175" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -5023,16 +5019,16 @@
         <v>176</v>
       </c>
       <c r="B176" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C176" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D176" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E176" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5040,16 +5036,16 @@
         <v>177</v>
       </c>
       <c r="B177" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C177" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D177" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E177" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5057,16 +5053,16 @@
         <v>178</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C178" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D178" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E178" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -5074,16 +5070,16 @@
         <v>179</v>
       </c>
       <c r="B179" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C179" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D179" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E179" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5091,16 +5087,16 @@
         <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C180" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D180" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E180" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -5108,102 +5104,102 @@
         <v>181</v>
       </c>
       <c r="B181" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C181" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D181" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E181" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B182" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C182" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="E182" s="4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="4" t="s">
+      <c r="B182" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B183" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C183" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="184" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="4" t="s">
+      <c r="B183" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B184" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C184" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="4" t="s">
+      <c r="B184" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B185" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C185" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="4" t="s">
+      <c r="B185" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B186" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C186" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="4" t="s">
+      <c r="B186" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B187" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C187" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="4" t="s">
+      <c r="B187" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B188" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="C188" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D188" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E188" s="4" t="s">
-        <v>342</v>
+      <c r="B188" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5211,16 +5207,16 @@
         <v>189</v>
       </c>
       <c r="B189" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C189" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D189" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E189" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5228,33 +5224,33 @@
         <v>190</v>
       </c>
       <c r="B190" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C190" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D190" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E190" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B191" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="C191" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D191" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E191" s="4" t="s">
-        <v>342</v>
+      <c r="B191" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5262,101 +5258,101 @@
         <v>192</v>
       </c>
       <c r="B192" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C192" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D192" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E192" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B193" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B194" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="C193" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D193" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E193" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B194" s="4" t="s">
+      <c r="C194" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B195" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="C194" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D194" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E194" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="B195" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="C195" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D195" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E195" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="4" t="s">
+      <c r="C195" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B196" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="C196" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D196" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E196" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="4" t="s">
+      <c r="B196" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B197" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="C197" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D197" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E197" s="4" t="s">
-        <v>342</v>
+      <c r="B197" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5364,33 +5360,33 @@
         <v>198</v>
       </c>
       <c r="B198" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C198" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D198" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E198" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="B199" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C199" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D199" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E199" s="4" t="s">
-        <v>342</v>
+      <c r="B199" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="200" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5398,13 +5394,16 @@
         <v>200</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>212</v>
+        <v>408</v>
       </c>
       <c r="C200" s="3" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="201" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5412,30 +5411,33 @@
         <v>201</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>212</v>
+        <v>407</v>
       </c>
       <c r="C201" s="3" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B202" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="C202" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D202" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E202" s="4" t="s">
-        <v>342</v>
+      <c r="B202" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5443,84 +5445,84 @@
         <v>203</v>
       </c>
       <c r="B203" t="s">
+        <v>251</v>
+      </c>
+      <c r="C203" t="s">
+        <v>343</v>
+      </c>
+      <c r="D203" t="s">
+        <v>333</v>
+      </c>
+      <c r="E203" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B204" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C203" t="s">
-        <v>344</v>
-      </c>
-      <c r="D203" t="s">
-        <v>334</v>
-      </c>
-      <c r="E203" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B204" s="4" t="s">
+      <c r="C204" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B205" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="C204" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D204" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E204" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="B205" s="4" t="s">
+      <c r="C205" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B206" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C205" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D205" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E205" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="B206" s="4" t="s">
+      <c r="C206" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B207" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C206" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D206" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E206" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="B207" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="C207" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D207" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E207" s="4" t="s">
-        <v>342</v>
+      <c r="C207" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5528,58 +5530,58 @@
         <v>208</v>
       </c>
       <c r="B208" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C208" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E208" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B209" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="C209" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D209" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="E209" s="4" t="s">
-        <v>342</v>
+      <c r="B209" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>210</v>
       </c>
-      <c r="B210" s="4" t="s">
-        <v>246</v>
+      <c r="B210" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="C210" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E210" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>211</v>
       </c>
-      <c r="B211" s="4" t="s">
-        <v>246</v>
+      <c r="B211" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="C211" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E211" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>